<commit_message>
solved problem 28 in java/python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ns102894\Documents\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986BC61C-6BB2-4D2E-806C-652AB04E4CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711A6CA9-61DF-46C4-A0CA-8DFB2AC7CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="269">
   <si>
     <t>Problem Type</t>
   </si>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
   <dimension ref="A2:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,6 +1639,9 @@
       <c r="L9" t="s">
         <v>54</v>
       </c>
+      <c r="M9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>

<commit_message>
solved more java problems
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ns102894\Documents\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF15CE8-72BE-49BF-824E-1766082EF405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8A4D0F-275A-4C2A-A94E-8A42D188E80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="274">
   <si>
     <t>Problem Type</t>
   </si>
@@ -843,6 +843,21 @@
   </si>
   <si>
     <t>23 minutes</t>
+  </si>
+  <si>
+    <t>Problem Number</t>
+  </si>
+  <si>
+    <t>58-Length of Last Word</t>
+  </si>
+  <si>
+    <t>One Pass Loop</t>
+  </si>
+  <si>
+    <t>80- Remove Duplicates from Sorted Array II</t>
+  </si>
+  <si>
+    <t>Two pointer one pass</t>
   </si>
 </sst>
 </file>
@@ -987,10 +1002,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:W72" totalsRowShown="0">
-  <autoFilter ref="A2:W72" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X73" totalsRowShown="0">
+  <autoFilter ref="A2:X73" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
+    <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
     <tableColumn id="2" xr3:uid="{BBE78027-130D-438F-9D41-F2EC289220D4}" name="Name of Problem"/>
     <tableColumn id="3" xr3:uid="{2F950F82-E676-4857-A451-61E7207BDECB}" name="Difficulty"/>
     <tableColumn id="22" xr3:uid="{660A3F6C-C7B3-4793-AD09-2CCA7A046093}" name="My algorithm"/>
@@ -1315,2084 +1331,2209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:W72"/>
+  <dimension ref="A2:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" customWidth="1"/>
-    <col min="14" max="14" width="44.42578125" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" customWidth="1"/>
-    <col min="16" max="16" width="27.85546875" customWidth="1"/>
-    <col min="17" max="28" width="12" customWidth="1"/>
+    <col min="1" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="48.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" customWidth="1"/>
+    <col min="15" max="15" width="44.42578125" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" customWidth="1"/>
+    <col min="18" max="29" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>58</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>207</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>13</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>14</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>15</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>16</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>17</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
       <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>
       <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" t="s">
+      <c r="L4" s="1"/>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
       </c>
       <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" t="s">
+      <c r="L5" s="1"/>
+      <c r="M5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
       </c>
       <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>51</v>
       </c>
       <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>57</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>62</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>54</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3">
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
         <v>69</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>71</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>72</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>72</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>169</v>
+      </c>
+      <c r="C12" t="s">
         <v>76</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
       <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>46</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>78</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>73</v>
       </c>
-      <c r="J12"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K12"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>80</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
       <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
         <v>82</v>
       </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
       <c r="F13" t="s">
         <v>83</v>
       </c>
-      <c r="H13" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="1"/>
-      <c r="L13" t="s">
+      <c r="L13" s="1"/>
+      <c r="M13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>85</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
       <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
         <v>86</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>87</v>
       </c>
-      <c r="F14" t="s">
-        <v>83</v>
-      </c>
       <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
         <v>88</v>
       </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" t="s">
         <v>73</v>
       </c>
-      <c r="K14" s="1"/>
-      <c r="L14" t="s">
+      <c r="L14" s="1"/>
+      <c r="M14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>90</v>
       </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
       <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
         <v>92</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>93</v>
       </c>
-      <c r="F15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H15" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
         <v>92</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" t="s">
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>96</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
       <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
         <v>98</v>
-      </c>
-      <c r="E17" t="s">
-        <v>99</v>
       </c>
       <c r="F17" t="s">
         <v>99</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s">
         <v>99</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
       <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
         <v>103</v>
-      </c>
-      <c r="E18" t="s">
-        <v>104</v>
       </c>
       <c r="F18" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>109</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>108</v>
       </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
       <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
         <v>109</v>
-      </c>
-      <c r="E19" t="s">
-        <v>110</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
       </c>
-      <c r="I19" t="s">
+      <c r="G19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
       </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
       <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
         <v>113</v>
       </c>
-      <c r="E20" t="s">
-        <v>83</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" t="s">
+      <c r="L20" s="1"/>
+      <c r="M20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>115</v>
       </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
       <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
         <v>116</v>
       </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="1"/>
-      <c r="L21" t="s">
+      <c r="L21" s="1"/>
+      <c r="M21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>118</v>
       </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
       <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
         <v>119</v>
       </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" t="s">
+      <c r="L22" s="1"/>
+      <c r="M22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
       <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
         <v>122</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>46</v>
       </c>
-      <c r="F23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H23" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="1"/>
-      <c r="L23" t="s">
+      <c r="L23" s="1"/>
+      <c r="M23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>124</v>
       </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
       <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
         <v>125</v>
-      </c>
-      <c r="E24" t="s">
-        <v>126</v>
       </c>
       <c r="F24" t="s">
         <v>126</v>
       </c>
       <c r="G24" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" t="s">
         <v>125</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>126</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>129</v>
       </c>
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
       <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
         <v>128</v>
       </c>
-      <c r="E25" t="s">
-        <v>83</v>
-      </c>
       <c r="F25" t="s">
         <v>83</v>
       </c>
       <c r="G25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>131</v>
       </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
       <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
         <v>132</v>
       </c>
-      <c r="E26" t="s">
-        <v>83</v>
-      </c>
       <c r="F26" t="s">
         <v>83</v>
       </c>
-      <c r="H26" t="s">
-        <v>83</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="G26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>117</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>134</v>
       </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
       <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
         <v>135</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>138</v>
       </c>
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
       <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
         <v>139</v>
-      </c>
-      <c r="E28" t="s">
-        <v>72</v>
       </c>
       <c r="F28" t="s">
         <v>72</v>
       </c>
-      <c r="H28" t="s">
+      <c r="G28" t="s">
         <v>72</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="I28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
       <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
         <v>143</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>144</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>71</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>73</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" t="s">
-        <v>20</v>
-      </c>
       <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
         <v>147</v>
-      </c>
-      <c r="E30" t="s">
-        <v>148</v>
       </c>
       <c r="F30" t="s">
         <v>148</v>
       </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>148</v>
       </c>
       <c r="I30" t="s">
+        <v>148</v>
+      </c>
+      <c r="J30" t="s">
         <v>64</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K30" s="1"/>
-      <c r="L30" t="s">
+      <c r="L30" s="1"/>
+      <c r="M30" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>149</v>
       </c>
-      <c r="C31" t="s">
-        <v>20</v>
-      </c>
       <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
         <v>150</v>
       </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="L31" t="s">
+      <c r="F31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>153</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>154</v>
       </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
       <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
         <v>155</v>
       </c>
-      <c r="E32" t="s">
-        <v>83</v>
-      </c>
       <c r="F32" t="s">
         <v>83</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="G32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="M32" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>157</v>
       </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
       <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
         <v>158</v>
       </c>
-      <c r="E33" t="s">
-        <v>83</v>
-      </c>
       <c r="F33" t="s">
         <v>83</v>
       </c>
-      <c r="H33" t="s">
-        <v>83</v>
-      </c>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>159</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>160</v>
       </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
       <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
         <v>161</v>
       </c>
-      <c r="E34" t="s">
-        <v>83</v>
-      </c>
       <c r="F34" t="s">
         <v>83</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s">
         <v>83</v>
       </c>
       <c r="I34" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>163</v>
       </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
       <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
         <v>164</v>
       </c>
-      <c r="E35" t="s">
-        <v>83</v>
-      </c>
       <c r="F35" t="s">
         <v>83</v>
       </c>
       <c r="G35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>166</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>167</v>
       </c>
-      <c r="C36" t="s">
-        <v>20</v>
-      </c>
       <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
         <v>168</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>169</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>170</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>166</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>172</v>
       </c>
-      <c r="C37" t="s">
-        <v>20</v>
-      </c>
       <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
         <v>173</v>
       </c>
-      <c r="E37" t="s">
-        <v>83</v>
-      </c>
       <c r="F37" t="s">
         <v>83</v>
       </c>
       <c r="G37" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" t="s">
         <v>175</v>
       </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
       <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
         <v>30</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>176</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>178</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>180</v>
       </c>
-      <c r="C39" t="s">
-        <v>20</v>
-      </c>
       <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>181</v>
       </c>
-      <c r="E39" t="s">
-        <v>83</v>
-      </c>
       <c r="F39" t="s">
         <v>83</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39" t="s">
         <v>83</v>
       </c>
       <c r="I39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J39" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>184</v>
       </c>
-      <c r="C40" t="s">
-        <v>20</v>
-      </c>
       <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
         <v>185</v>
       </c>
-      <c r="E40" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="L40" t="s">
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="L40" s="1"/>
+      <c r="M40" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>265</v>
       </c>
-      <c r="C41" t="s">
-        <v>20</v>
-      </c>
       <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
         <v>173</v>
       </c>
-      <c r="E41" t="s">
-        <v>83</v>
-      </c>
       <c r="F41" t="s">
         <v>83</v>
       </c>
       <c r="G41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" t="s">
         <v>266</v>
       </c>
-      <c r="H41" t="s">
-        <v>83</v>
-      </c>
       <c r="I41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" t="s">
         <v>267</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K41" s="1"/>
-      <c r="L41" t="s">
+      <c r="L41" s="1"/>
+      <c r="M41" t="s">
         <v>268</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>271</v>
+      </c>
+      <c r="F42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" t="s">
+        <v>271</v>
+      </c>
+      <c r="I42" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L42" s="1"/>
+      <c r="M42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>187</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
         <v>188</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E43" t="s">
         <v>161</v>
       </c>
-      <c r="E42" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" t="s">
-        <v>83</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="F43" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:24" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44"/>
+      <c r="C44" t="s">
         <v>190</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>188</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E44" t="s">
         <v>60</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F44" t="s">
         <v>191</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G44" t="s">
         <v>192</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H44" t="s">
         <v>193</v>
       </c>
-      <c r="H43"/>
-      <c r="I43" t="s">
+      <c r="I44"/>
+      <c r="J44" t="s">
         <v>73</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M44" t="s">
         <v>75</v>
       </c>
-      <c r="M43"/>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43"/>
-      <c r="S43"/>
-      <c r="T43"/>
-      <c r="U43"/>
-      <c r="V43"/>
-      <c r="W43"/>
-    </row>
-    <row r="44" spans="1:23" ht="165" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+    </row>
+    <row r="45" spans="1:24" ht="165" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="F45" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12" t="s">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="L45" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="L44" s="11" t="s">
+      <c r="M45" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="M44" s="11" t="s">
+      <c r="N45" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-      <c r="T44" s="11"/>
-      <c r="U44" s="11"/>
-      <c r="V44" s="11"/>
-      <c r="W44" s="11"/>
-    </row>
-    <row r="45" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+    </row>
+    <row r="46" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>166</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46"/>
+      <c r="C46" t="s">
         <v>198</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>188</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E46" t="s">
         <v>166</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F46" t="s">
         <v>71</v>
       </c>
-      <c r="F45"/>
-      <c r="G45" t="s">
+      <c r="G46"/>
+      <c r="H46" t="s">
         <v>166</v>
       </c>
-      <c r="H45"/>
-      <c r="I45"/>
-      <c r="J45" s="1" t="s">
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K45" s="1"/>
-      <c r="L45" t="s">
+      <c r="L46" s="1"/>
+      <c r="M46" t="s">
         <v>34</v>
       </c>
-      <c r="M45"/>
-      <c r="N45"/>
-      <c r="O45"/>
-      <c r="P45"/>
-      <c r="Q45"/>
-      <c r="R45"/>
-      <c r="S45"/>
-      <c r="T45"/>
-      <c r="U45"/>
-      <c r="V45"/>
-      <c r="W45"/>
-    </row>
-    <row r="46" spans="1:23" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="M46" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" ht="135" x14ac:dyDescent="0.25">
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+    </row>
+    <row r="47" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="C47" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="M47" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="I48" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12" t="s">
+      <c r="J48" s="11"/>
+      <c r="K48" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="L48" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="M48" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="N48" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-    </row>
-    <row r="48" spans="1:23" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>19</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49"/>
+      <c r="C49" t="s">
         <v>210</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>188</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E49" t="s">
         <v>205</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F49" t="s">
         <v>211</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G49" t="s">
         <v>211</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H49" t="s">
         <v>205</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I49" t="s">
         <v>211</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J49" t="s">
         <v>64</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M49" t="s">
         <v>54</v>
       </c>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-    </row>
-    <row r="49" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+    </row>
+    <row r="50" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="G50" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="I50" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="J50" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="K50" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="L50" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-    </row>
-    <row r="50" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+    </row>
+    <row r="51" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>19</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C51" t="s">
         <v>218</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D51" t="s">
         <v>188</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E51" t="s">
         <v>219</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F51" t="s">
         <v>220</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G51" t="s">
         <v>220</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H51" t="s">
         <v>219</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I51" t="s">
         <v>220</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J51" t="s">
         <v>64</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M51" t="s">
         <v>54</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N51" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="90" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>215</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C52" t="s">
         <v>223</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D52" t="s">
         <v>188</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E52" t="s">
         <v>224</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F52" t="s">
         <v>225</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G52" t="s">
         <v>225</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H52" t="s">
         <v>224</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I52" t="s">
         <v>225</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J52" t="s">
         <v>64</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="90" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" t="s">
-        <v>227</v>
-      </c>
-      <c r="C52" t="s">
-        <v>188</v>
-      </c>
-      <c r="D52" t="s">
-        <v>228</v>
-      </c>
-      <c r="E52" t="s">
-        <v>71</v>
-      </c>
-      <c r="F52" t="s">
-        <v>71</v>
-      </c>
-      <c r="G52" t="s">
-        <v>228</v>
-      </c>
-      <c r="H52" t="s">
-        <v>71</v>
-      </c>
-      <c r="I52" t="s">
-        <v>64</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L52" t="s">
-        <v>75</v>
-      </c>
-      <c r="M52" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" ht="150" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>69</v>
       </c>
-      <c r="B53" t="s">
-        <v>230</v>
-      </c>
       <c r="C53" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D53" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="F53" t="s">
         <v>71</v>
       </c>
       <c r="G53" t="s">
+        <v>71</v>
+      </c>
+      <c r="H53" t="s">
+        <v>228</v>
+      </c>
+      <c r="I53" t="s">
+        <v>71</v>
+      </c>
+      <c r="J53" t="s">
+        <v>64</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N53" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="150" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s">
+        <v>230</v>
+      </c>
+      <c r="D54" t="s">
+        <v>231</v>
+      </c>
+      <c r="E54" t="s">
         <v>232</v>
       </c>
-      <c r="H53" t="s">
+      <c r="F54" t="s">
         <v>71</v>
       </c>
-      <c r="I53" t="s">
+      <c r="G54" t="s">
+        <v>71</v>
+      </c>
+      <c r="H54" t="s">
+        <v>232</v>
+      </c>
+      <c r="I54" t="s">
+        <v>71</v>
+      </c>
+      <c r="J54" t="s">
         <v>64</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M54" t="s">
         <v>75</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N54" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="135" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>234</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C55" t="s">
         <v>235</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D55" t="s">
         <v>188</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E55" t="s">
         <v>236</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F55" t="s">
         <v>237</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G55" t="s">
         <v>237</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H55" t="s">
         <v>238</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I55" t="s">
         <v>239</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J55" t="s">
         <v>64</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M55" t="s">
         <v>56</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:23" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>215</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56"/>
+      <c r="C56" t="s">
         <v>241</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D56" t="s">
         <v>188</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E56" t="s">
         <v>215</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F56" t="s">
         <v>242</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G56" t="s">
         <v>242</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H56" t="s">
         <v>215</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I56" t="s">
         <v>242</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J56" t="s">
         <v>64</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="L55" t="s">
+      <c r="M56" t="s">
         <v>56</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N56" t="s">
         <v>244</v>
       </c>
-      <c r="N55"/>
-      <c r="O55"/>
-      <c r="P55"/>
-      <c r="Q55"/>
-      <c r="R55"/>
-      <c r="S55"/>
-      <c r="T55"/>
-      <c r="U55"/>
-      <c r="V55"/>
-      <c r="W55"/>
-    </row>
-    <row r="56" spans="1:23" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="L56" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="M56" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" ht="210" x14ac:dyDescent="0.25">
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+      <c r="U56"/>
+      <c r="V56"/>
+      <c r="W56"/>
+      <c r="X56"/>
+    </row>
+    <row r="57" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="C57" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="N57" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="E58" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="F58" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="G58" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="H58" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="H57" s="11" t="s">
+      <c r="I58" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="I57" s="11" t="s">
+      <c r="J58" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J57" s="12" t="s">
+      <c r="K58" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K57" s="12" t="s">
+      <c r="L58" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="L57" s="11" t="s">
+      <c r="M58" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="M57" s="11" t="s">
+      <c r="N58" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
-      <c r="U57" s="11"/>
-      <c r="V57" s="11"/>
-      <c r="W57" s="11"/>
-    </row>
-    <row r="58" spans="1:23" ht="120" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" t="s">
-        <v>255</v>
-      </c>
-      <c r="C58" t="s">
-        <v>188</v>
-      </c>
-      <c r="D58" t="s">
-        <v>258</v>
-      </c>
-      <c r="E58" t="s">
-        <v>257</v>
-      </c>
-      <c r="F58" t="s">
-        <v>257</v>
-      </c>
-      <c r="G58" t="s">
-        <v>256</v>
-      </c>
-      <c r="H58" t="s">
-        <v>257</v>
-      </c>
-      <c r="I58" t="s">
-        <v>64</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="L58" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+      <c r="W58" s="11"/>
+      <c r="X58" s="11"/>
+    </row>
+    <row r="59" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>255</v>
+      </c>
+      <c r="D59" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" t="s">
+        <v>258</v>
+      </c>
+      <c r="F59" t="s">
+        <v>257</v>
+      </c>
+      <c r="G59" t="s">
+        <v>257</v>
+      </c>
+      <c r="H59" t="s">
+        <v>256</v>
+      </c>
+      <c r="I59" t="s">
+        <v>257</v>
+      </c>
+      <c r="J59" t="s">
+        <v>64</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="M59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
         <v>260</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D60" t="s">
         <v>188</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E60" t="s">
         <v>261</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F60" t="s">
         <v>262</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G60" t="s">
         <v>262</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H60" t="s">
         <v>261</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I60" t="s">
         <v>262</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J60" t="s">
         <v>64</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L60" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M60" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K60" s="1"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K61" s="1"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K62" s="1"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K63" s="1"/>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K64" s="1"/>
-    </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K65" s="1"/>
-    </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K66" s="1"/>
-    </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K67" s="1"/>
-    </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K68" s="1"/>
-    </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K70" s="1"/>
-    </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K71" s="1"/>
-    </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K72" s="1"/>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>272</v>
+      </c>
+      <c r="D61" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" t="s">
+        <v>273</v>
+      </c>
+      <c r="F61" t="s">
+        <v>220</v>
+      </c>
+      <c r="G61" t="s">
+        <v>220</v>
+      </c>
+      <c r="H61" t="s">
+        <v>220</v>
+      </c>
+      <c r="I61" t="s">
+        <v>220</v>
+      </c>
+      <c r="J61" t="s">
+        <v>64</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L61" s="1"/>
+      <c r="M61" t="s">
+        <v>264</v>
+      </c>
+      <c r="N61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L65" s="1"/>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L67" s="1"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L69" s="1"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L71" s="1"/>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L72" s="1"/>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L73" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
solved problem 205 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ns102894\Documents\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8A4D0F-275A-4C2A-A94E-8A42D188E80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7D266B-2942-4E07-8D2F-C42D476FC381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="278">
   <si>
     <t>Problem Type</t>
   </si>
@@ -858,6 +858,18 @@
   </si>
   <si>
     <t>Two pointer one pass</t>
+  </si>
+  <si>
+    <t>205 - Isomorphic Strings</t>
+  </si>
+  <si>
+    <t>One pass loop, 2 hashmaps</t>
+  </si>
+  <si>
+    <t>The trick here is really with making sure you check both ways the mapping is the same, and not just one way.</t>
+  </si>
+  <si>
+    <t>35 minutes</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1014,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X73" totalsRowShown="0">
-  <autoFilter ref="A2:X73" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X74" totalsRowShown="0">
+  <autoFilter ref="A2:X74" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1331,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X73"/>
+  <dimension ref="A2:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,23 +2697,32 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>141</v>
+      </c>
+      <c r="B43">
+        <v>205</v>
       </c>
       <c r="C43" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
       <c r="D43" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
       <c r="F43" t="s">
         <v>83</v>
       </c>
       <c r="G43" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" t="s">
+        <v>275</v>
+      </c>
+      <c r="I43" t="s">
         <v>83</v>
       </c>
       <c r="J43" t="s">
@@ -2711,435 +2732,432 @@
         <v>73</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>189</v>
+        <v>276</v>
       </c>
       <c r="M43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="N43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44"/>
+        <v>48</v>
+      </c>
       <c r="C44" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D44" t="s">
         <v>188</v>
       </c>
       <c r="E44" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G44" t="s">
-        <v>192</v>
-      </c>
-      <c r="H44" t="s">
-        <v>193</v>
-      </c>
-      <c r="I44"/>
+        <v>83</v>
+      </c>
       <c r="J44" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45"/>
+      <c r="C45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G45" t="s">
+        <v>192</v>
+      </c>
+      <c r="H45" t="s">
+        <v>193</v>
+      </c>
+      <c r="I45"/>
+      <c r="J45" t="s">
+        <v>73</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M45" t="s">
         <v>75</v>
       </c>
-      <c r="N44"/>
-      <c r="O44"/>
-      <c r="P44"/>
-      <c r="Q44"/>
-      <c r="R44"/>
-      <c r="S44"/>
-      <c r="T44"/>
-      <c r="U44"/>
-      <c r="V44"/>
-      <c r="W44"/>
-      <c r="X44"/>
-    </row>
-    <row r="45" spans="1:24" ht="165" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+    </row>
+    <row r="46" spans="1:24" ht="165" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11" t="s">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E46" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F46" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="12" t="s">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="L46" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M45" s="11" t="s">
+      <c r="M46" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N45" s="11" t="s">
+      <c r="N46" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
-      <c r="V45" s="11"/>
-      <c r="W45" s="11"/>
-      <c r="X45" s="11"/>
-    </row>
-    <row r="46" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+    </row>
+    <row r="47" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>166</v>
       </c>
-      <c r="B46"/>
-      <c r="C46" t="s">
+      <c r="B47"/>
+      <c r="C47" t="s">
         <v>198</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>188</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>166</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>71</v>
       </c>
-      <c r="G46"/>
-      <c r="H46" t="s">
+      <c r="G47"/>
+      <c r="H47" t="s">
         <v>166</v>
       </c>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46" s="1" t="s">
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L46" s="1"/>
-      <c r="M46" t="s">
+      <c r="L47" s="1"/>
+      <c r="M47" t="s">
         <v>34</v>
       </c>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-    </row>
-    <row r="47" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M47" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N47" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+    </row>
+    <row r="48" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="11"/>
       <c r="C48" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J48" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K48" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M48" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N48" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="11"/>
-      <c r="W48" s="11"/>
-      <c r="X48" s="11"/>
-    </row>
-    <row r="49" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    </row>
+    <row r="49" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B49"/>
-      <c r="C49" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+    </row>
+    <row r="50" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50"/>
+      <c r="C50" t="s">
         <v>210</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>188</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>205</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>211</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>211</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H50" t="s">
         <v>205</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I50" t="s">
         <v>211</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J50" t="s">
         <v>64</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M50" t="s">
         <v>54</v>
       </c>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-      <c r="S49"/>
-      <c r="T49"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-    </row>
-    <row r="50" spans="1:24" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+    </row>
+    <row r="51" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E51" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G50" s="11" t="s">
+      <c r="G51" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H51" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I50" s="11" t="s">
+      <c r="I51" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="J51" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K51" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="L51" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-    </row>
-    <row r="51" spans="1:24" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+    </row>
+    <row r="52" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>19</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>218</v>
-      </c>
-      <c r="D51" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" t="s">
-        <v>219</v>
-      </c>
-      <c r="F51" t="s">
-        <v>220</v>
-      </c>
-      <c r="G51" t="s">
-        <v>220</v>
-      </c>
-      <c r="H51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I51" t="s">
-        <v>220</v>
-      </c>
-      <c r="J51" t="s">
-        <v>64</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M51" t="s">
-        <v>54</v>
-      </c>
-      <c r="N51" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="90" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>215</v>
-      </c>
-      <c r="C52" t="s">
-        <v>223</v>
       </c>
       <c r="D52" t="s">
         <v>188</v>
       </c>
       <c r="E52" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F52" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G52" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H52" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I52" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J52" t="s">
         <v>64</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M52" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="N52" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C53" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D53" t="s">
         <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G53" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I53" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J53" t="s">
         <v>64</v>
@@ -3148,27 +3166,24 @@
         <v>73</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M53" t="s">
-        <v>75</v>
-      </c>
-      <c r="N53" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="150" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D54" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F54" t="s">
         <v>71</v>
@@ -3177,7 +3192,7 @@
         <v>71</v>
       </c>
       <c r="H54" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I54" t="s">
         <v>71</v>
@@ -3189,7 +3204,7 @@
         <v>73</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M54" t="s">
         <v>75</v>
@@ -3198,162 +3213,161 @@
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
       <c r="C55" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D55" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E55" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F55" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G55" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="H55" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I55" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="J55" t="s">
         <v>64</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M55" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="N55" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>215</v>
-      </c>
-      <c r="B56"/>
+        <v>234</v>
+      </c>
       <c r="C56" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D56" t="s">
         <v>188</v>
       </c>
       <c r="E56" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F56" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G56" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H56" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I56" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J56" t="s">
         <v>64</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M56" t="s">
         <v>56</v>
       </c>
       <c r="N56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57"/>
+      <c r="C57" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57" t="s">
+        <v>242</v>
+      </c>
+      <c r="G57" t="s">
+        <v>242</v>
+      </c>
+      <c r="H57" t="s">
+        <v>215</v>
+      </c>
+      <c r="I57" t="s">
+        <v>242</v>
+      </c>
+      <c r="J57" t="s">
+        <v>64</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M57" t="s">
+        <v>56</v>
+      </c>
+      <c r="N57" t="s">
         <v>244</v>
       </c>
-      <c r="O56"/>
-      <c r="P56"/>
-      <c r="Q56"/>
-      <c r="R56"/>
-      <c r="S56"/>
-      <c r="T56"/>
-      <c r="U56"/>
-      <c r="V56"/>
-      <c r="W56"/>
-      <c r="X56"/>
-    </row>
-    <row r="57" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M57" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N57" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+      <c r="U57"/>
+      <c r="V57"/>
+      <c r="W57"/>
+      <c r="X57"/>
+    </row>
+    <row r="58" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="11"/>
       <c r="C58" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J58" s="11" t="s">
         <v>64</v>
@@ -3362,128 +3376,129 @@
         <v>73</v>
       </c>
       <c r="L58" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M58" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N58" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
-      <c r="T58" s="11"/>
-      <c r="U58" s="11"/>
-      <c r="V58" s="11"/>
-      <c r="W58" s="11"/>
-      <c r="X58" s="11"/>
-    </row>
-    <row r="59" spans="1:24" ht="120" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    </row>
+    <row r="59" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C59" t="s">
-        <v>255</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B59" s="11"/>
+      <c r="C59" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E59" t="s">
-        <v>258</v>
-      </c>
-      <c r="F59" t="s">
-        <v>257</v>
-      </c>
-      <c r="G59" t="s">
-        <v>257</v>
-      </c>
-      <c r="H59" t="s">
-        <v>256</v>
-      </c>
-      <c r="I59" t="s">
-        <v>257</v>
-      </c>
-      <c r="J59" t="s">
+      <c r="E59" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M59" t="s">
+      <c r="K59" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M59" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+      <c r="N59" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
+      <c r="V59" s="11"/>
+      <c r="W59" s="11"/>
+      <c r="X59" s="11"/>
+    </row>
+    <row r="60" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D60" t="s">
         <v>188</v>
       </c>
       <c r="E60" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F60" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G60" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H60" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I60" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J60" t="s">
         <v>64</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M60" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
-      <c r="B61">
-        <v>80</v>
-      </c>
       <c r="C61" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D61" t="s">
         <v>188</v>
       </c>
       <c r="E61" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F61" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G61" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H61" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I61" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J61" t="s">
         <v>64</v>
@@ -3491,16 +3506,54 @@
       <c r="K61" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L61" s="1"/>
+      <c r="L61" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M61" t="s">
         <v>264</v>
       </c>
-      <c r="N61" t="s">
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62">
+        <v>80</v>
+      </c>
+      <c r="C62" t="s">
+        <v>272</v>
+      </c>
+      <c r="D62" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" t="s">
+        <v>273</v>
+      </c>
+      <c r="F62" t="s">
+        <v>220</v>
+      </c>
+      <c r="G62" t="s">
+        <v>220</v>
+      </c>
+      <c r="H62" t="s">
+        <v>220</v>
+      </c>
+      <c r="I62" t="s">
+        <v>220</v>
+      </c>
+      <c r="J62" t="s">
+        <v>64</v>
+      </c>
+      <c r="K62" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L62" s="1"/>
+      <c r="M62" t="s">
+        <v>264</v>
+      </c>
+      <c r="N62" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L63" s="1"/>
@@ -3534,6 +3587,9 @@
     </row>
     <row r="73" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L73" s="1"/>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
solved rotate array 189 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ns102894\Documents\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7D266B-2942-4E07-8D2F-C42D476FC381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B695C-0EA0-41FA-963A-5320BA7D235D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="283">
   <si>
     <t>Problem Type</t>
   </si>
@@ -870,6 +870,22 @@
   </si>
   <si>
     <t>35 minutes</t>
+  </si>
+  <si>
+    <t>189-Rotate Array</t>
+  </si>
+  <si>
+    <t>Cyclic replacement</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Reverse Array</t>
+  </si>
+  <si>
+    <t>I spent a lot of time trying to come up with a cyclic approach which was really tricky to account for the edge cases.
+The trick to this problem was to relaize you can reverse the array, and then reverse the array 2 more times in 2 separate portions to obtain the end result</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
   <dimension ref="A2:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,6 +3233,9 @@
       <c r="A55" t="s">
         <v>69</v>
       </c>
+      <c r="B55">
+        <v>34</v>
+      </c>
       <c r="C55" t="s">
         <v>230</v>
       </c>
@@ -3258,6 +3277,9 @@
       <c r="A56" t="s">
         <v>234</v>
       </c>
+      <c r="B56">
+        <v>36</v>
+      </c>
       <c r="C56" t="s">
         <v>235</v>
       </c>
@@ -3299,7 +3321,9 @@
       <c r="A57" t="s">
         <v>215</v>
       </c>
-      <c r="B57"/>
+      <c r="B57">
+        <v>46</v>
+      </c>
       <c r="C57" t="s">
         <v>241</v>
       </c>
@@ -3351,6 +3375,9 @@
       <c r="A58" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="B58" s="11">
+        <v>48</v>
+      </c>
       <c r="C58" s="11" t="s">
         <v>245</v>
       </c>
@@ -3389,7 +3416,9 @@
       <c r="A59" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="11">
+        <v>49</v>
+      </c>
       <c r="C59" s="11" t="s">
         <v>249</v>
       </c>
@@ -3441,6 +3470,9 @@
       <c r="A60" t="s">
         <v>19</v>
       </c>
+      <c r="B60">
+        <v>54</v>
+      </c>
       <c r="C60" t="s">
         <v>255</v>
       </c>
@@ -3555,8 +3587,49 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="L63" s="1"/>
+    <row r="63" spans="1:24" ht="225" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63">
+        <v>189</v>
+      </c>
+      <c r="C63" t="s">
+        <v>278</v>
+      </c>
+      <c r="D63" t="s">
+        <v>188</v>
+      </c>
+      <c r="E63" t="s">
+        <v>279</v>
+      </c>
+      <c r="F63" t="s">
+        <v>280</v>
+      </c>
+      <c r="G63" t="s">
+        <v>83</v>
+      </c>
+      <c r="H63" t="s">
+        <v>281</v>
+      </c>
+      <c r="I63" t="s">
+        <v>220</v>
+      </c>
+      <c r="J63" t="s">
+        <v>64</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M63" t="s">
+        <v>114</v>
+      </c>
+      <c r="N63" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L64" s="1"/>

</xml_diff>

<commit_message>
Solved 252 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ns102894\Documents\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B695C-0EA0-41FA-963A-5320BA7D235D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA74C87-D7CD-4CAA-90AB-0950E4D35497}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="288">
   <si>
     <t>Problem Type</t>
   </si>
@@ -886,6 +886,21 @@
   <si>
     <t>I spent a lot of time trying to come up with a cyclic approach which was really tricky to account for the edge cases.
 The trick to this problem was to relaize you can reverse the array, and then reverse the array 2 more times in 2 separate portions to obtain the end result</t>
+  </si>
+  <si>
+    <t>252 - Meeting Rooms</t>
+  </si>
+  <si>
+    <t>Sort, then iterate</t>
+  </si>
+  <si>
+    <t>O(nlogn) time, O(n) memory</t>
+  </si>
+  <si>
+    <t>O(nlogn) time</t>
+  </si>
+  <si>
+    <t>O(n) memory</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1045,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X74" totalsRowShown="0">
-  <autoFilter ref="A2:X74" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X75" totalsRowShown="0">
+  <autoFilter ref="A2:X75" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1359,34 +1374,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X74"/>
+  <dimension ref="A2:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" customWidth="1"/>
+    <col min="1" max="2" width="37.453125" customWidth="1"/>
+    <col min="3" max="3" width="52.7265625" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" customWidth="1"/>
+    <col min="5" max="5" width="45.81640625" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.26953125" customWidth="1"/>
+    <col min="8" max="8" width="48.1796875" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="34.7265625" customWidth="1"/>
     <col min="11" max="11" width="26" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" customWidth="1"/>
-    <col min="15" max="15" width="44.42578125" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" customWidth="1"/>
-    <col min="17" max="17" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" customWidth="1"/>
+    <col min="13" max="13" width="25.81640625" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" customWidth="1"/>
+    <col min="15" max="15" width="44.453125" customWidth="1"/>
+    <col min="16" max="16" width="26.1796875" customWidth="1"/>
+    <col min="17" max="17" width="27.81640625" customWidth="1"/>
     <col min="18" max="29" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1498,7 +1513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1635,7 +1650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1670,7 +1685,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1711,7 +1726,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1750,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1770,7 +1785,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1804,7 +1819,7 @@
       <c r="K12"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1837,7 +1852,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1870,7 +1885,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1898,7 +1913,7 @@
       <c r="K15"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>91</v>
       </c>
@@ -1926,7 +1941,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1958,7 +1973,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1990,7 +2005,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -2022,7 +2037,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2046,7 +2061,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2085,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2094,7 +2109,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2127,7 +2142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2165,7 +2180,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2197,7 +2212,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -2255,7 +2270,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -2287,7 +2302,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -2325,7 +2340,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -2359,7 +2374,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2406,7 +2421,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2430,7 +2445,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>159</v>
       </c>
@@ -2465,7 +2480,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -2497,7 +2512,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>166</v>
       </c>
@@ -2523,7 +2538,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -2549,7 +2564,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
@@ -2579,7 +2594,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2614,7 +2629,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2635,7 +2650,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2674,7 +2689,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2713,7 +2728,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>141</v>
       </c>
@@ -2757,461 +2772,459 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="B44">
+        <v>252</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>283</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>161</v>
+        <v>284</v>
       </c>
       <c r="F44" t="s">
-        <v>83</v>
+        <v>285</v>
       </c>
       <c r="G44" t="s">
-        <v>83</v>
+        <v>286</v>
+      </c>
+      <c r="I44" t="s">
+        <v>287</v>
       </c>
       <c r="J44" t="s">
         <v>64</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="L44" s="1"/>
       <c r="M44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45"/>
+        <v>48</v>
+      </c>
       <c r="C45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D45" t="s">
         <v>188</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F45" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G45" t="s">
-        <v>192</v>
-      </c>
-      <c r="H45" t="s">
-        <v>193</v>
-      </c>
-      <c r="I45"/>
+        <v>83</v>
+      </c>
       <c r="J45" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L45" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46"/>
+      <c r="C46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" t="s">
+        <v>192</v>
+      </c>
+      <c r="H46" t="s">
+        <v>193</v>
+      </c>
+      <c r="I46"/>
+      <c r="J46" t="s">
+        <v>73</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L46" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M46" t="s">
         <v>75</v>
       </c>
-      <c r="N45"/>
-      <c r="O45"/>
-      <c r="P45"/>
-      <c r="Q45"/>
-      <c r="R45"/>
-      <c r="S45"/>
-      <c r="T45"/>
-      <c r="U45"/>
-      <c r="V45"/>
-      <c r="W45"/>
-      <c r="X45"/>
-    </row>
-    <row r="46" spans="1:24" ht="165" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+    </row>
+    <row r="47" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A47" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E47" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F47" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="12" t="s">
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L46" s="12" t="s">
+      <c r="L47" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M46" s="11" t="s">
+      <c r="M47" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N46" s="11" t="s">
+      <c r="N47" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
-      <c r="T46" s="11"/>
-      <c r="U46" s="11"/>
-      <c r="V46" s="11"/>
-      <c r="W46" s="11"/>
-      <c r="X46" s="11"/>
-    </row>
-    <row r="47" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+    </row>
+    <row r="48" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>166</v>
       </c>
-      <c r="B47"/>
-      <c r="C47" t="s">
+      <c r="B48"/>
+      <c r="C48" t="s">
         <v>198</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>188</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>166</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>71</v>
       </c>
-      <c r="G47"/>
-      <c r="H47" t="s">
+      <c r="G48"/>
+      <c r="H48" t="s">
         <v>166</v>
       </c>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47" s="1" t="s">
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L47" s="1"/>
-      <c r="M47" t="s">
+      <c r="L48" s="1"/>
+      <c r="M48" t="s">
         <v>34</v>
       </c>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-    </row>
-    <row r="48" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L48" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M48" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N48" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+    </row>
+    <row r="49" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="11"/>
       <c r="C49" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J49" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K49" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M49" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N49" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
-    </row>
-    <row r="50" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    </row>
+    <row r="50" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B50"/>
-      <c r="C50" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J50" s="11"/>
+      <c r="K50" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N50" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+    </row>
+    <row r="51" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51"/>
+      <c r="C51" t="s">
         <v>210</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>188</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>205</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>211</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>211</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>205</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I51" t="s">
         <v>211</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J51" t="s">
         <v>64</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M51" t="s">
         <v>54</v>
       </c>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50"/>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-    </row>
-    <row r="51" spans="1:24" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+    </row>
+    <row r="52" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11" t="s">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G52" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I51" s="11" t="s">
+      <c r="I52" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J51" s="11" t="s">
+      <c r="J52" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K51" s="12" t="s">
+      <c r="K52" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L51" s="12" t="s">
+      <c r="L52" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
-      <c r="X51" s="11"/>
-    </row>
-    <row r="52" spans="1:24" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+      <c r="U52" s="11"/>
+      <c r="V52" s="11"/>
+      <c r="W52" s="11"/>
+      <c r="X52" s="11"/>
+    </row>
+    <row r="53" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>218</v>
-      </c>
-      <c r="D52" t="s">
-        <v>188</v>
-      </c>
-      <c r="E52" t="s">
-        <v>219</v>
-      </c>
-      <c r="F52" t="s">
-        <v>220</v>
-      </c>
-      <c r="G52" t="s">
-        <v>220</v>
-      </c>
-      <c r="H52" t="s">
-        <v>219</v>
-      </c>
-      <c r="I52" t="s">
-        <v>220</v>
-      </c>
-      <c r="J52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M52" t="s">
-        <v>54</v>
-      </c>
-      <c r="N52" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" ht="90" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>215</v>
-      </c>
-      <c r="C53" t="s">
-        <v>223</v>
       </c>
       <c r="D53" t="s">
         <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H53" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J53" t="s">
         <v>64</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="N53" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C54" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D54" t="s">
         <v>188</v>
       </c>
       <c r="E54" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F54" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G54" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H54" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I54" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J54" t="s">
         <v>64</v>
@@ -3220,30 +3233,24 @@
         <v>73</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M54" t="s">
-        <v>75</v>
-      </c>
-      <c r="N54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="150" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>69</v>
       </c>
-      <c r="B55">
-        <v>34</v>
-      </c>
       <c r="C55" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D55" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F55" t="s">
         <v>71</v>
@@ -3252,7 +3259,7 @@
         <v>71</v>
       </c>
       <c r="H55" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I55" t="s">
         <v>71</v>
@@ -3264,7 +3271,7 @@
         <v>73</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M55" t="s">
         <v>75</v>
@@ -3273,172 +3280,172 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
       <c r="B56">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D56" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E56" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F56" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G56" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="H56" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I56" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="J56" t="s">
         <v>64</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M56" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="N56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B57">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D57" t="s">
         <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F57" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G57" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H57" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I57" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J57" t="s">
         <v>64</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M57" t="s">
         <v>56</v>
       </c>
       <c r="N57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58">
+        <v>46</v>
+      </c>
+      <c r="C58" t="s">
+        <v>241</v>
+      </c>
+      <c r="D58" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" t="s">
+        <v>242</v>
+      </c>
+      <c r="G58" t="s">
+        <v>242</v>
+      </c>
+      <c r="H58" t="s">
+        <v>215</v>
+      </c>
+      <c r="I58" t="s">
+        <v>242</v>
+      </c>
+      <c r="J58" t="s">
+        <v>64</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M58" t="s">
+        <v>56</v>
+      </c>
+      <c r="N58" t="s">
         <v>244</v>
       </c>
-      <c r="O57"/>
-      <c r="P57"/>
-      <c r="Q57"/>
-      <c r="R57"/>
-      <c r="S57"/>
-      <c r="T57"/>
-      <c r="U57"/>
-      <c r="V57"/>
-      <c r="W57"/>
-      <c r="X57"/>
-    </row>
-    <row r="58" spans="1:24" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="11">
-        <v>48</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J58" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L58" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M58" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N58" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="T58"/>
+      <c r="U58"/>
+      <c r="V58"/>
+      <c r="W58"/>
+      <c r="X58"/>
+    </row>
+    <row r="59" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J59" s="11" t="s">
         <v>64</v>
@@ -3447,131 +3454,134 @@
         <v>73</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M59" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N59" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
-      <c r="T59" s="11"/>
-      <c r="U59" s="11"/>
-      <c r="V59" s="11"/>
-      <c r="W59" s="11"/>
-      <c r="X59" s="11"/>
-    </row>
-    <row r="60" spans="1:24" ht="120" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    </row>
+    <row r="60" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A60" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B60">
-        <v>54</v>
-      </c>
-      <c r="C60" t="s">
-        <v>255</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="B60" s="11">
+        <v>49</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D60" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E60" t="s">
-        <v>258</v>
-      </c>
-      <c r="F60" t="s">
-        <v>257</v>
-      </c>
-      <c r="G60" t="s">
-        <v>257</v>
-      </c>
-      <c r="H60" t="s">
-        <v>256</v>
-      </c>
-      <c r="I60" t="s">
-        <v>257</v>
-      </c>
-      <c r="J60" t="s">
+      <c r="E60" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J60" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M60" t="s">
+      <c r="K60" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L60" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M60" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="61" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+      <c r="N60" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+    </row>
+    <row r="61" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>19</v>
       </c>
+      <c r="B61">
+        <v>54</v>
+      </c>
       <c r="C61" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D61" t="s">
         <v>188</v>
       </c>
       <c r="E61" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F61" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G61" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H61" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I61" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J61" t="s">
         <v>64</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M61" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" ht="174" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>19</v>
       </c>
-      <c r="B62">
-        <v>80</v>
-      </c>
       <c r="C62" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
       </c>
       <c r="E62" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F62" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G62" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H62" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I62" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J62" t="s">
         <v>64</v>
@@ -3579,38 +3589,37 @@
       <c r="K62" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L62" s="1"/>
+      <c r="L62" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M62" t="s">
         <v>264</v>
       </c>
-      <c r="N62" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>19</v>
       </c>
       <c r="B63">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D63" t="s">
         <v>188</v>
       </c>
       <c r="E63" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F63" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G63" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H63" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I63" t="s">
         <v>220</v>
@@ -3619,50 +3628,92 @@
         <v>64</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L63" s="1"/>
       <c r="M63" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N63" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <v>189</v>
+      </c>
+      <c r="C64" t="s">
+        <v>278</v>
+      </c>
+      <c r="D64" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" t="s">
+        <v>279</v>
+      </c>
+      <c r="F64" t="s">
+        <v>280</v>
+      </c>
+      <c r="G64" t="s">
+        <v>83</v>
+      </c>
+      <c r="H64" t="s">
+        <v>281</v>
+      </c>
+      <c r="I64" t="s">
+        <v>220</v>
+      </c>
+      <c r="J64" t="s">
+        <v>64</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M64" t="s">
+        <v>114</v>
+      </c>
+      <c r="N64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L74" s="1"/>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 100 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA74C87-D7CD-4CAA-90AB-0950E4D35497}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB81686B-7517-4E58-B46E-B59671E23C1F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="-28920" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="290">
   <si>
     <t>Problem Type</t>
   </si>
@@ -901,6 +901,12 @@
   </si>
   <si>
     <t>O(n) memory</t>
+  </si>
+  <si>
+    <t>100 - Same Tree</t>
+  </si>
+  <si>
+    <t>Iterative BFS</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1001,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1021,6 +1027,9 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1044,9 +1053,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X75" totalsRowShown="0">
-  <autoFilter ref="A2:X75" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X76" totalsRowShown="0">
+  <autoFilter ref="A2:X76" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1374,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X75"/>
+  <dimension ref="A2:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1913,152 +1926,157 @@
       <c r="K15"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>288</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>289</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="H16" s="13"/>
       <c r="I16" t="s">
-        <v>46</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K16"/>
       <c r="L16" s="1"/>
       <c r="M16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>96</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>97</v>
       </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
         <v>98</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>99</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>99</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>99</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
         <v>103</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>104</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>104</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J19" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>109</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
         <v>109</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>110</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>110</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>64</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" t="s">
-        <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M20" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -2066,13 +2084,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
         <v>83</v>
@@ -2082,21 +2100,21 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
         <v>83</v>
@@ -2106,124 +2124,116 @@
       </c>
       <c r="L22" s="1"/>
       <c r="M22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" t="s">
         <v>83</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
-        <v>124</v>
+      <c r="C24" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H24" t="s">
-        <v>125</v>
+        <v>83</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="I24" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="L24" s="1"/>
       <c r="M24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="H25" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="I25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" t="s">
+        <v>64</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F26" t="s">
         <v>83</v>
@@ -2231,423 +2241,434 @@
       <c r="G26" t="s">
         <v>83</v>
       </c>
-      <c r="I26" t="s">
-        <v>83</v>
+      <c r="H26" t="s">
+        <v>128</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M26" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>83</v>
+      </c>
+      <c r="G27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" t="s">
+        <v>83</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
         <v>72</v>
       </c>
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" t="s">
-        <v>72</v>
-      </c>
       <c r="K28" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="M28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
         <v>143</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>144</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>71</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>71</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J30" t="s">
         <v>73</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" t="s">
-        <v>146</v>
-      </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" t="s">
-        <v>148</v>
-      </c>
-      <c r="G30" t="s">
-        <v>148</v>
-      </c>
-      <c r="I30" t="s">
-        <v>148</v>
-      </c>
-      <c r="J30" t="s">
-        <v>64</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L30" s="1"/>
+      <c r="L30" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="M30" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
+      <c r="A31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
         <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>148</v>
+      </c>
+      <c r="G31" t="s">
+        <v>148</v>
+      </c>
+      <c r="I31" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" s="1"/>
+      <c r="M32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="33" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>153</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>154</v>
       </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
         <v>155</v>
       </c>
-      <c r="F32" t="s">
-        <v>83</v>
-      </c>
-      <c r="G32" t="s">
-        <v>83</v>
-      </c>
-      <c r="L32" s="1" t="s">
+      <c r="F33" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M32" s="10" t="s">
+      <c r="M33" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>157</v>
       </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
         <v>158</v>
       </c>
-      <c r="F33" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="F34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>159</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>160</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
         <v>161</v>
       </c>
-      <c r="F34" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>83</v>
-      </c>
-      <c r="I34" t="s">
-        <v>83</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="F35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M35" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>163</v>
       </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
         <v>164</v>
       </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>166</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>167</v>
       </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
         <v>168</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>169</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>170</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>166</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>19</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>172</v>
       </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
         <v>173</v>
       </c>
-      <c r="F37" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" t="s">
         <v>23</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" t="s">
         <v>175</v>
       </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>30</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>176</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I39" t="s">
         <v>178</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="M38" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>180</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J39" t="s">
-        <v>64</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M39" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D40" t="s">
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F40" t="s">
         <v>83</v>
       </c>
-      <c r="L40" s="1"/>
+      <c r="G40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40" t="s">
+        <v>64</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M40" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.35">
@@ -2655,55 +2676,34 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>265</v>
+        <v>184</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F41" t="s">
         <v>83</v>
-      </c>
-      <c r="G41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H41" t="s">
-        <v>266</v>
-      </c>
-      <c r="I41" t="s">
-        <v>83</v>
-      </c>
-      <c r="J41" t="s">
-        <v>267</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" t="s">
-        <v>268</v>
-      </c>
-      <c r="N41" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
-      <c r="B42">
-        <v>58</v>
-      </c>
       <c r="C42" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
         <v>83</v>
@@ -2712,37 +2712,40 @@
         <v>83</v>
       </c>
       <c r="H42" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I42" t="s">
         <v>83</v>
       </c>
       <c r="J42" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B43">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F43" t="s">
         <v>83</v>
@@ -2751,7 +2754,7 @@
         <v>83</v>
       </c>
       <c r="H43" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I43" t="s">
         <v>83</v>
@@ -2762,507 +2765,508 @@
       <c r="K43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="L43" s="1"/>
       <c r="M43" t="s">
-        <v>277</v>
-      </c>
-      <c r="N43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B44">
-        <v>252</v>
+        <v>205</v>
       </c>
       <c r="C44" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="F44" t="s">
-        <v>285</v>
+        <v>83</v>
       </c>
       <c r="G44" t="s">
-        <v>286</v>
+        <v>83</v>
+      </c>
+      <c r="H44" t="s">
+        <v>275</v>
       </c>
       <c r="I44" t="s">
-        <v>287</v>
+        <v>83</v>
       </c>
       <c r="J44" t="s">
         <v>64</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="M44" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="N44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="B45">
+        <v>252</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
+        <v>283</v>
       </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>161</v>
+        <v>284</v>
       </c>
       <c r="F45" t="s">
-        <v>83</v>
+        <v>285</v>
       </c>
       <c r="G45" t="s">
-        <v>83</v>
+        <v>286</v>
+      </c>
+      <c r="I45" t="s">
+        <v>287</v>
       </c>
       <c r="J45" t="s">
         <v>64</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="L45" s="1"/>
       <c r="M45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46"/>
+        <v>48</v>
+      </c>
       <c r="C46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D46" t="s">
         <v>188</v>
       </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F46" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G46" t="s">
-        <v>192</v>
-      </c>
-      <c r="H46" t="s">
-        <v>193</v>
-      </c>
-      <c r="I46"/>
+        <v>83</v>
+      </c>
       <c r="J46" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L46" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47"/>
+      <c r="C47" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" t="s">
+        <v>191</v>
+      </c>
+      <c r="G47" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" t="s">
+        <v>193</v>
+      </c>
+      <c r="I47"/>
+      <c r="J47" t="s">
+        <v>73</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M47" t="s">
         <v>75</v>
       </c>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-    </row>
-    <row r="47" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+    </row>
+    <row r="48" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A48" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11" t="s">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="12" t="s">
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L47" s="12" t="s">
+      <c r="L48" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M48" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N47" s="11" t="s">
+      <c r="N48" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-      <c r="X47" s="11"/>
-    </row>
-    <row r="48" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>166</v>
       </c>
-      <c r="B48"/>
-      <c r="C48" t="s">
+      <c r="B49"/>
+      <c r="C49" t="s">
         <v>198</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>188</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>166</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>71</v>
       </c>
-      <c r="G48"/>
-      <c r="H48" t="s">
+      <c r="G49"/>
+      <c r="H49" t="s">
         <v>166</v>
       </c>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48" s="1" t="s">
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L48" s="1"/>
-      <c r="M48" t="s">
+      <c r="L49" s="1"/>
+      <c r="M49" t="s">
         <v>34</v>
       </c>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-      <c r="X48"/>
-    </row>
-    <row r="49" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A49" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K49" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L49" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M49" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N49" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+    </row>
+    <row r="50" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="11"/>
       <c r="C50" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J50" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K50" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M50" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N50" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-    </row>
-    <row r="51" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    </row>
+    <row r="51" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B51"/>
-      <c r="C51" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J51" s="11"/>
+      <c r="K51" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M51" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+    </row>
+    <row r="52" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52"/>
+      <c r="C52" t="s">
         <v>210</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>188</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>205</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>211</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G52" t="s">
         <v>211</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H52" t="s">
         <v>205</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>211</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J52" t="s">
         <v>64</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M52" t="s">
         <v>54</v>
       </c>
-      <c r="N51"/>
-      <c r="O51"/>
-      <c r="P51"/>
-      <c r="Q51"/>
-      <c r="R51"/>
-      <c r="S51"/>
-      <c r="T51"/>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-    </row>
-    <row r="52" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+    </row>
+    <row r="53" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11" t="s">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G53" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H52" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I52" s="11" t="s">
+      <c r="I53" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J52" s="11" t="s">
+      <c r="J53" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K52" s="12" t="s">
+      <c r="K53" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L52" s="12" t="s">
+      <c r="L53" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
-      <c r="X52" s="11"/>
-    </row>
-    <row r="53" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="11"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="11"/>
+      <c r="W53" s="11"/>
+      <c r="X53" s="11"/>
+    </row>
+    <row r="54" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>19</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>218</v>
-      </c>
-      <c r="D53" t="s">
-        <v>188</v>
-      </c>
-      <c r="E53" t="s">
-        <v>219</v>
-      </c>
-      <c r="F53" t="s">
-        <v>220</v>
-      </c>
-      <c r="G53" t="s">
-        <v>220</v>
-      </c>
-      <c r="H53" t="s">
-        <v>219</v>
-      </c>
-      <c r="I53" t="s">
-        <v>220</v>
-      </c>
-      <c r="J53" t="s">
-        <v>64</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M53" t="s">
-        <v>54</v>
-      </c>
-      <c r="N53" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>215</v>
-      </c>
-      <c r="C54" t="s">
-        <v>223</v>
       </c>
       <c r="D54" t="s">
         <v>188</v>
       </c>
       <c r="E54" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F54" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G54" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H54" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I54" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J54" t="s">
         <v>64</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M54" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="N54" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D55" t="s">
         <v>188</v>
       </c>
       <c r="E55" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F55" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G55" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H55" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I55" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J55" t="s">
         <v>64</v>
@@ -3271,30 +3275,24 @@
         <v>73</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M55" t="s">
-        <v>75</v>
-      </c>
-      <c r="N55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>69</v>
       </c>
-      <c r="B56">
-        <v>34</v>
-      </c>
       <c r="C56" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D56" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E56" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F56" t="s">
         <v>71</v>
@@ -3303,7 +3301,7 @@
         <v>71</v>
       </c>
       <c r="H56" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I56" t="s">
         <v>71</v>
@@ -3315,7 +3313,7 @@
         <v>73</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M56" t="s">
         <v>75</v>
@@ -3326,170 +3324,170 @@
     </row>
     <row r="57" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
       <c r="B57">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D57" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E57" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F57" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G57" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="H57" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I57" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="J57" t="s">
         <v>64</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M57" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="N57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B58">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D58" t="s">
         <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F58" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G58" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H58" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I58" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J58" t="s">
         <v>64</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M58" t="s">
         <v>56</v>
       </c>
       <c r="N58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59">
+        <v>46</v>
+      </c>
+      <c r="C59" t="s">
+        <v>241</v>
+      </c>
+      <c r="D59" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F59" t="s">
+        <v>242</v>
+      </c>
+      <c r="G59" t="s">
+        <v>242</v>
+      </c>
+      <c r="H59" t="s">
+        <v>215</v>
+      </c>
+      <c r="I59" t="s">
+        <v>242</v>
+      </c>
+      <c r="J59" t="s">
+        <v>64</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M59" t="s">
+        <v>56</v>
+      </c>
+      <c r="N59" t="s">
         <v>244</v>
       </c>
-      <c r="O58"/>
-      <c r="P58"/>
-      <c r="Q58"/>
-      <c r="R58"/>
-      <c r="S58"/>
-      <c r="T58"/>
-      <c r="U58"/>
-      <c r="V58"/>
-      <c r="W58"/>
-      <c r="X58"/>
-    </row>
-    <row r="59" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A59" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="11">
-        <v>48</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M59" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N59" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59"/>
+    </row>
+    <row r="60" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J60" s="11" t="s">
         <v>64</v>
@@ -3498,131 +3496,134 @@
         <v>73</v>
       </c>
       <c r="L60" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N60" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="11"/>
-      <c r="S60" s="11"/>
-      <c r="T60" s="11"/>
-      <c r="U60" s="11"/>
-      <c r="V60" s="11"/>
-      <c r="W60" s="11"/>
-      <c r="X60" s="11"/>
-    </row>
-    <row r="61" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    </row>
+    <row r="61" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A61" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B61">
-        <v>54</v>
-      </c>
-      <c r="C61" t="s">
-        <v>255</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B61" s="11">
+        <v>49</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E61" t="s">
-        <v>258</v>
-      </c>
-      <c r="F61" t="s">
-        <v>257</v>
-      </c>
-      <c r="G61" t="s">
-        <v>257</v>
-      </c>
-      <c r="H61" t="s">
-        <v>256</v>
-      </c>
-      <c r="I61" t="s">
-        <v>257</v>
-      </c>
-      <c r="J61" t="s">
+      <c r="E61" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J61" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M61" t="s">
+      <c r="K61" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L61" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M61" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="N61" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="T61" s="11"/>
+      <c r="U61" s="11"/>
+      <c r="V61" s="11"/>
+      <c r="W61" s="11"/>
+      <c r="X61" s="11"/>
+    </row>
+    <row r="62" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>19</v>
       </c>
+      <c r="B62">
+        <v>54</v>
+      </c>
       <c r="C62" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
       </c>
       <c r="E62" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F62" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G62" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H62" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I62" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J62" t="s">
         <v>64</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M62" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" ht="174" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>19</v>
       </c>
-      <c r="B63">
-        <v>80</v>
-      </c>
       <c r="C63" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D63" t="s">
         <v>188</v>
       </c>
       <c r="E63" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F63" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G63" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H63" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I63" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J63" t="s">
         <v>64</v>
@@ -3630,38 +3631,37 @@
       <c r="K63" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L63" s="1"/>
+      <c r="L63" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M63" t="s">
         <v>264</v>
       </c>
-      <c r="N63" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>19</v>
       </c>
       <c r="B64">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D64" t="s">
         <v>188</v>
       </c>
       <c r="E64" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F64" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G64" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H64" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I64" t="s">
         <v>220</v>
@@ -3670,50 +3670,92 @@
         <v>64</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L64" s="1"/>
       <c r="M64" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N64" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>189</v>
+      </c>
+      <c r="C65" t="s">
+        <v>278</v>
+      </c>
+      <c r="D65" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65" t="s">
+        <v>279</v>
+      </c>
+      <c r="F65" t="s">
+        <v>280</v>
+      </c>
+      <c r="G65" t="s">
+        <v>83</v>
+      </c>
+      <c r="H65" t="s">
+        <v>281</v>
+      </c>
+      <c r="I65" t="s">
+        <v>220</v>
+      </c>
+      <c r="J65" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M65" t="s">
+        <v>114</v>
+      </c>
+      <c r="N65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L75" s="1"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 70 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB81686B-7517-4E58-B46E-B59671E23C1F}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FF3439E-89CA-4A0C-A353-D931B34858DF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="57480" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="292">
   <si>
     <t>Problem Type</t>
   </si>
@@ -907,6 +907,12 @@
   </si>
   <si>
     <t>Iterative BFS</t>
+  </si>
+  <si>
+    <t>392-Is Subsequence</t>
+  </si>
+  <si>
+    <t>8 minutes</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1033,7 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,8 +1064,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X76" totalsRowShown="0">
-  <autoFilter ref="A2:X76" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X77" totalsRowShown="0">
+  <autoFilter ref="A2:X77" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1387,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X76"/>
+  <dimension ref="A2:X77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2675,21 +2681,36 @@
       <c r="A41" t="s">
         <v>19</v>
       </c>
+      <c r="B41">
+        <v>392</v>
+      </c>
       <c r="C41" t="s">
-        <v>184</v>
+        <v>290</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F41" t="s">
         <v>83</v>
+      </c>
+      <c r="G41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.35">
@@ -2697,55 +2718,34 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>265</v>
+        <v>184</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F42" t="s">
         <v>83</v>
-      </c>
-      <c r="G42" t="s">
-        <v>83</v>
-      </c>
-      <c r="H42" t="s">
-        <v>266</v>
-      </c>
-      <c r="I42" t="s">
-        <v>83</v>
-      </c>
-      <c r="J42" t="s">
-        <v>267</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" t="s">
-        <v>268</v>
-      </c>
-      <c r="N42" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
-      <c r="B43">
-        <v>58</v>
-      </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="F43" t="s">
         <v>83</v>
@@ -2754,37 +2754,40 @@
         <v>83</v>
       </c>
       <c r="H43" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I43" t="s">
         <v>83</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B44">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
@@ -2793,7 +2796,7 @@
         <v>83</v>
       </c>
       <c r="H44" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I44" t="s">
         <v>83</v>
@@ -2804,507 +2807,508 @@
       <c r="K44" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="L44" s="1"/>
+      <c r="M44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45">
+        <v>205</v>
+      </c>
+      <c r="C45" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" t="s">
+        <v>275</v>
+      </c>
+      <c r="I45" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="M44" t="s">
-        <v>277</v>
-      </c>
-      <c r="N44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45">
-        <v>252</v>
-      </c>
-      <c r="C45" t="s">
-        <v>283</v>
-      </c>
-      <c r="D45" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" t="s">
-        <v>284</v>
-      </c>
-      <c r="F45" t="s">
-        <v>285</v>
-      </c>
-      <c r="G45" t="s">
-        <v>286</v>
-      </c>
-      <c r="I45" t="s">
-        <v>287</v>
-      </c>
-      <c r="J45" t="s">
-        <v>64</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L45" s="1"/>
       <c r="M45" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="N45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <v>252</v>
+      </c>
+      <c r="C46" t="s">
+        <v>283</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>284</v>
+      </c>
+      <c r="F46" t="s">
+        <v>285</v>
+      </c>
+      <c r="G46" t="s">
+        <v>286</v>
+      </c>
+      <c r="I46" t="s">
+        <v>287</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L46" s="1"/>
+      <c r="M46" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>187</v>
-      </c>
-      <c r="D46" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" t="s">
-        <v>83</v>
-      </c>
-      <c r="G46" t="s">
-        <v>83</v>
-      </c>
-      <c r="J46" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47"/>
-      <c r="C47" t="s">
-        <v>190</v>
       </c>
       <c r="D47" t="s">
         <v>188</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F47" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G47" t="s">
-        <v>192</v>
-      </c>
-      <c r="H47" t="s">
-        <v>193</v>
-      </c>
-      <c r="I47"/>
+        <v>83</v>
+      </c>
       <c r="J47" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" t="s">
+        <v>191</v>
+      </c>
+      <c r="G48" t="s">
+        <v>192</v>
+      </c>
+      <c r="H48" t="s">
+        <v>193</v>
+      </c>
+      <c r="I48"/>
+      <c r="J48" t="s">
+        <v>73</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M48" t="s">
         <v>75</v>
       </c>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-    </row>
-    <row r="48" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A48" s="11" t="s">
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+    </row>
+    <row r="49" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E49" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="12" t="s">
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="L49" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M48" s="11" t="s">
+      <c r="M49" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N48" s="11" t="s">
+      <c r="N49" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="11"/>
-      <c r="W48" s="11"/>
-      <c r="X48" s="11"/>
-    </row>
-    <row r="49" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+    </row>
+    <row r="50" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>166</v>
       </c>
-      <c r="B49"/>
-      <c r="C49" t="s">
+      <c r="B50"/>
+      <c r="C50" t="s">
         <v>198</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>188</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>166</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>71</v>
       </c>
-      <c r="G49"/>
-      <c r="H49" t="s">
+      <c r="G50"/>
+      <c r="H50" t="s">
         <v>166</v>
       </c>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L49" s="1"/>
-      <c r="M49" t="s">
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L50" s="1"/>
+      <c r="M50" t="s">
         <v>34</v>
       </c>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-      <c r="S49"/>
-      <c r="T49"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-    </row>
-    <row r="50" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A50" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N50" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+    </row>
+    <row r="51" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="11"/>
       <c r="C51" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J51" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K51" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M51" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N51" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
-      <c r="X51" s="11"/>
-    </row>
-    <row r="52" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    </row>
+    <row r="52" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A52" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B52"/>
-      <c r="C52" t="s">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J52" s="11"/>
+      <c r="K52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+      <c r="U52" s="11"/>
+      <c r="V52" s="11"/>
+      <c r="W52" s="11"/>
+      <c r="X52" s="11"/>
+    </row>
+    <row r="53" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53"/>
+      <c r="C53" t="s">
         <v>210</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>188</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>205</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>211</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>211</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>205</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>211</v>
       </c>
-      <c r="J52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="1" t="s">
+      <c r="J53" t="s">
+        <v>64</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M53" t="s">
         <v>54</v>
       </c>
-      <c r="N52"/>
-      <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
-      <c r="S52"/>
-      <c r="T52"/>
-      <c r="U52"/>
-      <c r="V52"/>
-      <c r="W52"/>
-      <c r="X52"/>
-    </row>
-    <row r="53" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="11" t="s">
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+      <c r="V53"/>
+      <c r="W53"/>
+      <c r="X53"/>
+    </row>
+    <row r="54" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11" t="s">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E54" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G54" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I53" s="11" t="s">
+      <c r="I54" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J53" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K53" s="12" t="s">
+      <c r="J54" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K54" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L53" s="12" t="s">
+      <c r="L54" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
-      <c r="V53" s="11"/>
-      <c r="W53" s="11"/>
-      <c r="X53" s="11"/>
-    </row>
-    <row r="54" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="11"/>
+      <c r="U54" s="11"/>
+      <c r="V54" s="11"/>
+      <c r="W54" s="11"/>
+      <c r="X54" s="11"/>
+    </row>
+    <row r="55" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>19</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>218</v>
-      </c>
-      <c r="D54" t="s">
-        <v>188</v>
-      </c>
-      <c r="E54" t="s">
-        <v>219</v>
-      </c>
-      <c r="F54" t="s">
-        <v>220</v>
-      </c>
-      <c r="G54" t="s">
-        <v>220</v>
-      </c>
-      <c r="H54" t="s">
-        <v>219</v>
-      </c>
-      <c r="I54" t="s">
-        <v>220</v>
-      </c>
-      <c r="J54" t="s">
-        <v>64</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M54" t="s">
-        <v>54</v>
-      </c>
-      <c r="N54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>215</v>
-      </c>
-      <c r="C55" t="s">
-        <v>223</v>
       </c>
       <c r="D55" t="s">
         <v>188</v>
       </c>
       <c r="E55" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H55" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J55" t="s">
         <v>64</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="N55" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C56" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D56" t="s">
         <v>188</v>
       </c>
       <c r="E56" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G56" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H56" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I56" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J56" t="s">
         <v>64</v>
@@ -3313,30 +3317,24 @@
         <v>73</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M56" t="s">
-        <v>75</v>
-      </c>
-      <c r="N56" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>69</v>
       </c>
-      <c r="B57">
-        <v>34</v>
-      </c>
       <c r="C57" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D57" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F57" t="s">
         <v>71</v>
@@ -3345,7 +3343,7 @@
         <v>71</v>
       </c>
       <c r="H57" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I57" t="s">
         <v>71</v>
@@ -3357,7 +3355,7 @@
         <v>73</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M57" t="s">
         <v>75</v>
@@ -3368,170 +3366,170 @@
     </row>
     <row r="58" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58">
+        <v>34</v>
+      </c>
+      <c r="C58" t="s">
+        <v>230</v>
+      </c>
+      <c r="D58" t="s">
+        <v>231</v>
+      </c>
+      <c r="E58" t="s">
+        <v>232</v>
+      </c>
+      <c r="F58" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" t="s">
+        <v>232</v>
+      </c>
+      <c r="I58" t="s">
+        <v>71</v>
+      </c>
+      <c r="J58" t="s">
+        <v>64</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M58" t="s">
+        <v>75</v>
+      </c>
+      <c r="N58" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>234</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>36</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>235</v>
-      </c>
-      <c r="D58" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" t="s">
-        <v>236</v>
-      </c>
-      <c r="F58" t="s">
-        <v>237</v>
-      </c>
-      <c r="G58" t="s">
-        <v>237</v>
-      </c>
-      <c r="H58" t="s">
-        <v>238</v>
-      </c>
-      <c r="I58" t="s">
-        <v>239</v>
-      </c>
-      <c r="J58" t="s">
-        <v>64</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M58" t="s">
-        <v>56</v>
-      </c>
-      <c r="N58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>215</v>
-      </c>
-      <c r="B59">
-        <v>46</v>
-      </c>
-      <c r="C59" t="s">
-        <v>241</v>
       </c>
       <c r="D59" t="s">
         <v>188</v>
       </c>
       <c r="E59" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F59" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G59" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H59" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J59" t="s">
         <v>64</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M59" t="s">
         <v>56</v>
       </c>
       <c r="N59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>215</v>
+      </c>
+      <c r="B60">
+        <v>46</v>
+      </c>
+      <c r="C60" t="s">
+        <v>241</v>
+      </c>
+      <c r="D60" t="s">
+        <v>188</v>
+      </c>
+      <c r="E60" t="s">
+        <v>215</v>
+      </c>
+      <c r="F60" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" t="s">
+        <v>242</v>
+      </c>
+      <c r="H60" t="s">
+        <v>215</v>
+      </c>
+      <c r="I60" t="s">
+        <v>242</v>
+      </c>
+      <c r="J60" t="s">
+        <v>64</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M60" t="s">
+        <v>56</v>
+      </c>
+      <c r="N60" t="s">
         <v>244</v>
       </c>
-      <c r="O59"/>
-      <c r="P59"/>
-      <c r="Q59"/>
-      <c r="R59"/>
-      <c r="S59"/>
-      <c r="T59"/>
-      <c r="U59"/>
-      <c r="V59"/>
-      <c r="W59"/>
-      <c r="X59"/>
-    </row>
-    <row r="60" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A60" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="11">
-        <v>48</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J60" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M60" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N60" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+    </row>
+    <row r="61" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J61" s="11" t="s">
         <v>64</v>
@@ -3540,131 +3538,134 @@
         <v>73</v>
       </c>
       <c r="L61" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M61" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N61" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="11"/>
-      <c r="T61" s="11"/>
-      <c r="U61" s="11"/>
-      <c r="V61" s="11"/>
-      <c r="W61" s="11"/>
-      <c r="X61" s="11"/>
-    </row>
-    <row r="62" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    </row>
+    <row r="62" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A62" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B62">
-        <v>54</v>
-      </c>
-      <c r="C62" t="s">
-        <v>255</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B62" s="11">
+        <v>49</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E62" t="s">
-        <v>258</v>
-      </c>
-      <c r="F62" t="s">
-        <v>257</v>
-      </c>
-      <c r="G62" t="s">
-        <v>257</v>
-      </c>
-      <c r="H62" t="s">
-        <v>256</v>
-      </c>
-      <c r="I62" t="s">
-        <v>257</v>
-      </c>
-      <c r="J62" t="s">
-        <v>64</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M62" t="s">
+      <c r="E62" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J62" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K62" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L62" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M62" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="N62" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="T62" s="11"/>
+      <c r="U62" s="11"/>
+      <c r="V62" s="11"/>
+      <c r="W62" s="11"/>
+      <c r="X62" s="11"/>
+    </row>
+    <row r="63" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>19</v>
       </c>
+      <c r="B63">
+        <v>54</v>
+      </c>
       <c r="C63" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D63" t="s">
         <v>188</v>
       </c>
       <c r="E63" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F63" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G63" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H63" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I63" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J63" t="s">
         <v>64</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M63" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="174" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>19</v>
       </c>
-      <c r="B64">
-        <v>80</v>
-      </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D64" t="s">
         <v>188</v>
       </c>
       <c r="E64" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F64" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G64" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H64" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I64" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J64" t="s">
         <v>64</v>
@@ -3672,38 +3673,37 @@
       <c r="K64" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L64" s="1"/>
+      <c r="L64" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M64" t="s">
         <v>264</v>
       </c>
-      <c r="N64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>19</v>
       </c>
       <c r="B65">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D65" t="s">
         <v>188</v>
       </c>
       <c r="E65" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F65" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G65" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H65" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I65" t="s">
         <v>220</v>
@@ -3712,20 +3712,59 @@
         <v>64</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L65" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L65" s="1"/>
       <c r="M65" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N65" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L66" s="1"/>
+    <row r="66" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66">
+        <v>189</v>
+      </c>
+      <c r="C66" t="s">
+        <v>278</v>
+      </c>
+      <c r="D66" t="s">
+        <v>188</v>
+      </c>
+      <c r="E66" t="s">
+        <v>279</v>
+      </c>
+      <c r="F66" t="s">
+        <v>280</v>
+      </c>
+      <c r="G66" t="s">
+        <v>83</v>
+      </c>
+      <c r="H66" t="s">
+        <v>281</v>
+      </c>
+      <c r="I66" t="s">
+        <v>220</v>
+      </c>
+      <c r="J66" t="s">
+        <v>64</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M66" t="s">
+        <v>114</v>
+      </c>
+      <c r="N66" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L67" s="1"/>
@@ -3756,6 +3795,9 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L76" s="1"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L77" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 226 in java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FF3439E-89CA-4A0C-A353-D931B34858DF}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7C48A0-820B-4B1F-A8D6-62CD9556A261}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21040" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="295">
   <si>
     <t>Problem Type</t>
   </si>
@@ -913,6 +913,15 @@
   </si>
   <si>
     <t>8 minutes</t>
+  </si>
+  <si>
+    <t>226-Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>BFS Iterative que , swap current nodes</t>
+  </si>
+  <si>
+    <t>O(n), O(n) time</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1073,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X77" totalsRowShown="0">
-  <autoFilter ref="A2:X77" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X78" totalsRowShown="0">
+  <autoFilter ref="A2:X78" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1393,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X77"/>
+  <dimension ref="A2:X78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2443,255 +2452,244 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33">
+        <v>226</v>
+      </c>
+      <c r="C33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F33" t="s">
+        <v>294</v>
+      </c>
+      <c r="G33" t="s">
+        <v>294</v>
+      </c>
+      <c r="L33" s="1"/>
+      <c r="M33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>153</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>154</v>
       </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
         <v>155</v>
       </c>
-      <c r="F33" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33" s="1" t="s">
+      <c r="F34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M33" s="10" t="s">
+      <c r="M34" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>157</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
         <v>158</v>
       </c>
-      <c r="F34" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>83</v>
-      </c>
-      <c r="I34" t="s">
-        <v>83</v>
-      </c>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="F35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" t="s">
+        <v>83</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>159</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>160</v>
       </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
         <v>161</v>
       </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35" t="s">
-        <v>83</v>
-      </c>
-      <c r="J35" t="s">
-        <v>64</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" t="s">
+        <v>83</v>
+      </c>
+      <c r="J36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M36" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>163</v>
       </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
         <v>164</v>
       </c>
-      <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>83</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>166</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>167</v>
       </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
         <v>168</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>169</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>170</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>166</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>172</v>
       </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>173</v>
       </c>
-      <c r="F38" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" t="s">
-        <v>83</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H39" t="s">
         <v>23</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" t="s">
+      <c r="B40" s="3"/>
+      <c r="C40" t="s">
         <v>175</v>
       </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
         <v>30</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>176</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I40" t="s">
         <v>178</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L39" s="1" t="s">
+      <c r="K40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M40" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>180</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" t="s">
-        <v>181</v>
-      </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" t="s">
-        <v>83</v>
-      </c>
-      <c r="I40" t="s">
-        <v>83</v>
-      </c>
-      <c r="J40" t="s">
-        <v>64</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="M40" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B41">
-        <v>392</v>
-      </c>
       <c r="C41" t="s">
-        <v>290</v>
+        <v>180</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F41" t="s">
         <v>83</v>
@@ -2708,86 +2706,82 @@
       <c r="K41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L41" s="1"/>
+      <c r="L41" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M41" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
+      <c r="B42">
+        <v>392</v>
+      </c>
       <c r="C42" t="s">
-        <v>184</v>
+        <v>290</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
         <v>83</v>
+      </c>
+      <c r="G42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I42" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" t="s">
+        <v>64</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>265</v>
+        <v>184</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F43" t="s">
         <v>83</v>
-      </c>
-      <c r="G43" t="s">
-        <v>83</v>
-      </c>
-      <c r="H43" t="s">
-        <v>266</v>
-      </c>
-      <c r="I43" t="s">
-        <v>83</v>
-      </c>
-      <c r="J43" t="s">
-        <v>267</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" t="s">
-        <v>268</v>
-      </c>
-      <c r="N43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B44">
-        <v>58</v>
-      </c>
       <c r="C44" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
@@ -2796,37 +2790,40 @@
         <v>83</v>
       </c>
       <c r="H44" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I44" t="s">
         <v>83</v>
       </c>
       <c r="J44" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B45">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F45" t="s">
         <v>83</v>
@@ -2835,7 +2832,7 @@
         <v>83</v>
       </c>
       <c r="H45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I45" t="s">
         <v>83</v>
@@ -2846,507 +2843,508 @@
       <c r="K45" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="L45" s="1"/>
+      <c r="M45" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46">
+        <v>205</v>
+      </c>
+      <c r="C46" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>275</v>
+      </c>
+      <c r="F46" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L46" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="M45" t="s">
-        <v>277</v>
-      </c>
-      <c r="N45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46">
-        <v>252</v>
-      </c>
-      <c r="C46" t="s">
-        <v>283</v>
-      </c>
-      <c r="D46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46" t="s">
-        <v>284</v>
-      </c>
-      <c r="F46" t="s">
-        <v>285</v>
-      </c>
-      <c r="G46" t="s">
-        <v>286</v>
-      </c>
-      <c r="I46" t="s">
-        <v>287</v>
-      </c>
-      <c r="J46" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L46" s="1"/>
       <c r="M46" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="N46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47">
+        <v>252</v>
+      </c>
+      <c r="C47" t="s">
+        <v>283</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>284</v>
+      </c>
+      <c r="F47" t="s">
+        <v>285</v>
+      </c>
+      <c r="G47" t="s">
+        <v>286</v>
+      </c>
+      <c r="I47" t="s">
+        <v>287</v>
+      </c>
+      <c r="J47" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L47" s="1"/>
+      <c r="M47" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>187</v>
-      </c>
-      <c r="D47" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" t="s">
-        <v>161</v>
-      </c>
-      <c r="F47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G47" t="s">
-        <v>83</v>
-      </c>
-      <c r="J47" t="s">
-        <v>64</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48"/>
-      <c r="C48" t="s">
-        <v>190</v>
       </c>
       <c r="D48" t="s">
         <v>188</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F48" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G48" t="s">
-        <v>192</v>
-      </c>
-      <c r="H48" t="s">
-        <v>193</v>
-      </c>
-      <c r="I48"/>
+        <v>83</v>
+      </c>
       <c r="J48" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49"/>
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" t="s">
+        <v>191</v>
+      </c>
+      <c r="G49" t="s">
+        <v>192</v>
+      </c>
+      <c r="H49" t="s">
+        <v>193</v>
+      </c>
+      <c r="I49"/>
+      <c r="J49" t="s">
+        <v>73</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M49" t="s">
         <v>75</v>
       </c>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-      <c r="X48"/>
-    </row>
-    <row r="49" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A49" s="11" t="s">
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+    </row>
+    <row r="50" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="12" t="s">
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L49" s="12" t="s">
+      <c r="L50" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M49" s="11" t="s">
+      <c r="M50" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N49" s="11" t="s">
+      <c r="N50" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
-    </row>
-    <row r="50" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+    </row>
+    <row r="51" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>166</v>
       </c>
-      <c r="B50"/>
-      <c r="C50" t="s">
+      <c r="B51"/>
+      <c r="C51" t="s">
         <v>198</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>188</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>166</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>71</v>
       </c>
-      <c r="G50"/>
-      <c r="H50" t="s">
+      <c r="G51"/>
+      <c r="H51" t="s">
         <v>166</v>
       </c>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L50" s="1"/>
-      <c r="M50" t="s">
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L51" s="1"/>
+      <c r="M51" t="s">
         <v>34</v>
       </c>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50"/>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-    </row>
-    <row r="51" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I51" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M51" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N51" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+    </row>
+    <row r="52" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="11"/>
       <c r="C52" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J52" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K52" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L52" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M52" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N52" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
-      <c r="X52" s="11"/>
-    </row>
-    <row r="53" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    </row>
+    <row r="53" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B53"/>
-      <c r="C53" t="s">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J53" s="11"/>
+      <c r="K53" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M53" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="11"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="11"/>
+      <c r="W53" s="11"/>
+      <c r="X53" s="11"/>
+    </row>
+    <row r="54" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54"/>
+      <c r="C54" t="s">
         <v>210</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>188</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>205</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>211</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>211</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>205</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I54" t="s">
         <v>211</v>
       </c>
-      <c r="J53" t="s">
-        <v>64</v>
-      </c>
-      <c r="K53" s="1" t="s">
+      <c r="J54" t="s">
+        <v>64</v>
+      </c>
+      <c r="K54" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M54" t="s">
         <v>54</v>
       </c>
-      <c r="N53"/>
-      <c r="O53"/>
-      <c r="P53"/>
-      <c r="Q53"/>
-      <c r="R53"/>
-      <c r="S53"/>
-      <c r="T53"/>
-      <c r="U53"/>
-      <c r="V53"/>
-      <c r="W53"/>
-      <c r="X53"/>
-    </row>
-    <row r="54" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="11" t="s">
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+      <c r="U54"/>
+      <c r="V54"/>
+      <c r="W54"/>
+      <c r="X54"/>
+    </row>
+    <row r="55" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11" t="s">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H55" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I54" s="11" t="s">
+      <c r="I55" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J54" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K54" s="12" t="s">
+      <c r="J55" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K55" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L54" s="12" t="s">
+      <c r="L55" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-      <c r="S54" s="11"/>
-      <c r="T54" s="11"/>
-      <c r="U54" s="11"/>
-      <c r="V54" s="11"/>
-      <c r="W54" s="11"/>
-      <c r="X54" s="11"/>
-    </row>
-    <row r="55" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="11"/>
+      <c r="U55" s="11"/>
+      <c r="V55" s="11"/>
+      <c r="W55" s="11"/>
+      <c r="X55" s="11"/>
+    </row>
+    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>19</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>218</v>
-      </c>
-      <c r="D55" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" t="s">
-        <v>219</v>
-      </c>
-      <c r="F55" t="s">
-        <v>220</v>
-      </c>
-      <c r="G55" t="s">
-        <v>220</v>
-      </c>
-      <c r="H55" t="s">
-        <v>219</v>
-      </c>
-      <c r="I55" t="s">
-        <v>220</v>
-      </c>
-      <c r="J55" t="s">
-        <v>64</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M55" t="s">
-        <v>54</v>
-      </c>
-      <c r="N55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>215</v>
-      </c>
-      <c r="C56" t="s">
-        <v>223</v>
       </c>
       <c r="D56" t="s">
         <v>188</v>
       </c>
       <c r="E56" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F56" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G56" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H56" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I56" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J56" t="s">
         <v>64</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="N56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C57" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D57" t="s">
         <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F57" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G57" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H57" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I57" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J57" t="s">
         <v>64</v>
@@ -3355,30 +3353,24 @@
         <v>73</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M57" t="s">
-        <v>75</v>
-      </c>
-      <c r="N57" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>69</v>
       </c>
-      <c r="B58">
-        <v>34</v>
-      </c>
       <c r="C58" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D58" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F58" t="s">
         <v>71</v>
@@ -3387,7 +3379,7 @@
         <v>71</v>
       </c>
       <c r="H58" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I58" t="s">
         <v>71</v>
@@ -3399,7 +3391,7 @@
         <v>73</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M58" t="s">
         <v>75</v>
@@ -3410,170 +3402,170 @@
     </row>
     <row r="59" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59">
+        <v>34</v>
+      </c>
+      <c r="C59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" t="s">
+        <v>231</v>
+      </c>
+      <c r="E59" t="s">
+        <v>232</v>
+      </c>
+      <c r="F59" t="s">
+        <v>71</v>
+      </c>
+      <c r="G59" t="s">
+        <v>71</v>
+      </c>
+      <c r="H59" t="s">
+        <v>232</v>
+      </c>
+      <c r="I59" t="s">
+        <v>71</v>
+      </c>
+      <c r="J59" t="s">
+        <v>64</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M59" t="s">
+        <v>75</v>
+      </c>
+      <c r="N59" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>234</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>36</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>235</v>
-      </c>
-      <c r="D59" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" t="s">
-        <v>236</v>
-      </c>
-      <c r="F59" t="s">
-        <v>237</v>
-      </c>
-      <c r="G59" t="s">
-        <v>237</v>
-      </c>
-      <c r="H59" t="s">
-        <v>238</v>
-      </c>
-      <c r="I59" t="s">
-        <v>239</v>
-      </c>
-      <c r="J59" t="s">
-        <v>64</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M59" t="s">
-        <v>56</v>
-      </c>
-      <c r="N59" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>215</v>
-      </c>
-      <c r="B60">
-        <v>46</v>
-      </c>
-      <c r="C60" t="s">
-        <v>241</v>
       </c>
       <c r="D60" t="s">
         <v>188</v>
       </c>
       <c r="E60" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F60" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G60" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H60" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I60" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J60" t="s">
         <v>64</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M60" t="s">
         <v>56</v>
       </c>
       <c r="N60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61">
+        <v>46</v>
+      </c>
+      <c r="C61" t="s">
+        <v>241</v>
+      </c>
+      <c r="D61" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" t="s">
+        <v>215</v>
+      </c>
+      <c r="F61" t="s">
+        <v>242</v>
+      </c>
+      <c r="G61" t="s">
+        <v>242</v>
+      </c>
+      <c r="H61" t="s">
+        <v>215</v>
+      </c>
+      <c r="I61" t="s">
+        <v>242</v>
+      </c>
+      <c r="J61" t="s">
+        <v>64</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M61" t="s">
+        <v>56</v>
+      </c>
+      <c r="N61" t="s">
         <v>244</v>
       </c>
-      <c r="O60"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60"/>
-      <c r="T60"/>
-      <c r="U60"/>
-      <c r="V60"/>
-      <c r="W60"/>
-      <c r="X60"/>
-    </row>
-    <row r="61" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A61" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="11">
-        <v>48</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J61" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L61" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M61" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N61" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+      <c r="U61"/>
+      <c r="V61"/>
+      <c r="W61"/>
+      <c r="X61"/>
+    </row>
+    <row r="62" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J62" s="11" t="s">
         <v>64</v>
@@ -3582,131 +3574,134 @@
         <v>73</v>
       </c>
       <c r="L62" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M62" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N62" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O62" s="11"/>
-      <c r="P62" s="11"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-      <c r="S62" s="11"/>
-      <c r="T62" s="11"/>
-      <c r="U62" s="11"/>
-      <c r="V62" s="11"/>
-      <c r="W62" s="11"/>
-      <c r="X62" s="11"/>
-    </row>
-    <row r="63" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    </row>
+    <row r="63" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A63" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B63">
-        <v>54</v>
-      </c>
-      <c r="C63" t="s">
-        <v>255</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B63" s="11">
+        <v>49</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D63" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E63" t="s">
-        <v>258</v>
-      </c>
-      <c r="F63" t="s">
-        <v>257</v>
-      </c>
-      <c r="G63" t="s">
-        <v>257</v>
-      </c>
-      <c r="H63" t="s">
-        <v>256</v>
-      </c>
-      <c r="I63" t="s">
-        <v>257</v>
-      </c>
-      <c r="J63" t="s">
-        <v>64</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M63" t="s">
+      <c r="E63" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L63" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M63" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="N63" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="11"/>
+      <c r="T63" s="11"/>
+      <c r="U63" s="11"/>
+      <c r="V63" s="11"/>
+      <c r="W63" s="11"/>
+      <c r="X63" s="11"/>
+    </row>
+    <row r="64" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>19</v>
       </c>
+      <c r="B64">
+        <v>54</v>
+      </c>
       <c r="C64" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D64" t="s">
         <v>188</v>
       </c>
       <c r="E64" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F64" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G64" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H64" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I64" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J64" t="s">
         <v>64</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M64" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>19</v>
       </c>
-      <c r="B65">
-        <v>80</v>
-      </c>
       <c r="C65" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D65" t="s">
         <v>188</v>
       </c>
       <c r="E65" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F65" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G65" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H65" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I65" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J65" t="s">
         <v>64</v>
@@ -3714,38 +3709,37 @@
       <c r="K65" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L65" s="1"/>
+      <c r="L65" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M65" t="s">
         <v>264</v>
       </c>
-      <c r="N65" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>19</v>
       </c>
       <c r="B66">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C66" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
       </c>
       <c r="E66" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F66" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G66" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H66" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I66" t="s">
         <v>220</v>
@@ -3754,20 +3748,59 @@
         <v>64</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L66" s="1"/>
       <c r="M66" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L67" s="1"/>
+    <row r="67" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <v>189</v>
+      </c>
+      <c r="C67" t="s">
+        <v>278</v>
+      </c>
+      <c r="D67" t="s">
+        <v>188</v>
+      </c>
+      <c r="E67" t="s">
+        <v>279</v>
+      </c>
+      <c r="F67" t="s">
+        <v>280</v>
+      </c>
+      <c r="G67" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" t="s">
+        <v>281</v>
+      </c>
+      <c r="I67" t="s">
+        <v>220</v>
+      </c>
+      <c r="J67" t="s">
+        <v>64</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M67" t="s">
+        <v>114</v>
+      </c>
+      <c r="N67" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L68" s="1"/>
@@ -3798,6 +3831,9 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 572 in Java
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7C48A0-820B-4B1F-A8D6-62CD9556A261}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE0DFCE-497C-4E65-A82D-2D1DB9CF820F}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21040" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
+    <workbookView xWindow="57480" yWindow="15945" windowWidth="29040" windowHeight="15720" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="302">
   <si>
     <t>Problem Type</t>
   </si>
@@ -922,6 +922,27 @@
   </si>
   <si>
     <t>O(n), O(n) time</t>
+  </si>
+  <si>
+    <t>572 - SubTree Of Another Tree</t>
+  </si>
+  <si>
+    <t>DFS with nested subtree searches</t>
+  </si>
+  <si>
+    <t>O(N*M) time, O(N) memory</t>
+  </si>
+  <si>
+    <t>O(N + M)</t>
+  </si>
+  <si>
+    <t>Tree Hashing</t>
+  </si>
+  <si>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>Did nto fully solve this one or fully understand the optimal tree hashing solution</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1044,6 +1065,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1073,8 +1097,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X78" totalsRowShown="0">
-  <autoFilter ref="A2:X78" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X79" totalsRowShown="0">
+  <autoFilter ref="A2:X79" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1402,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X78"/>
+  <dimension ref="A2:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2770,60 +2794,54 @@
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" t="s">
-        <v>265</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" t="s">
-        <v>173</v>
-      </c>
-      <c r="F44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" t="s">
-        <v>266</v>
-      </c>
-      <c r="I44" t="s">
-        <v>83</v>
-      </c>
-      <c r="J44" t="s">
-        <v>267</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L44" s="1"/>
-      <c r="M44" t="s">
-        <v>268</v>
-      </c>
-      <c r="N44" t="s">
-        <v>105</v>
+    <row r="44" spans="1:14" s="10" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="10">
+        <v>572</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>19</v>
       </c>
-      <c r="B45">
-        <v>58</v>
-      </c>
       <c r="C45" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="F45" t="s">
         <v>83</v>
@@ -2832,37 +2850,40 @@
         <v>83</v>
       </c>
       <c r="H45" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I45" t="s">
         <v>83</v>
       </c>
       <c r="J45" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B46">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F46" t="s">
         <v>83</v>
@@ -2871,7 +2892,7 @@
         <v>83</v>
       </c>
       <c r="H46" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I46" t="s">
         <v>83</v>
@@ -2882,507 +2903,508 @@
       <c r="K46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="L46" s="1"/>
       <c r="M46" t="s">
-        <v>277</v>
-      </c>
-      <c r="N46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B47">
-        <v>252</v>
+        <v>205</v>
       </c>
       <c r="C47" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="F47" t="s">
-        <v>285</v>
+        <v>83</v>
       </c>
       <c r="G47" t="s">
-        <v>286</v>
+        <v>83</v>
+      </c>
+      <c r="H47" t="s">
+        <v>275</v>
       </c>
       <c r="I47" t="s">
-        <v>287</v>
+        <v>83</v>
       </c>
       <c r="J47" t="s">
         <v>64</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L47" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="M47" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="N47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="B48">
+        <v>252</v>
       </c>
       <c r="C48" t="s">
-        <v>187</v>
+        <v>283</v>
       </c>
       <c r="D48" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>161</v>
+        <v>284</v>
       </c>
       <c r="F48" t="s">
-        <v>83</v>
+        <v>285</v>
       </c>
       <c r="G48" t="s">
-        <v>83</v>
+        <v>286</v>
+      </c>
+      <c r="I48" t="s">
+        <v>287</v>
       </c>
       <c r="J48" t="s">
         <v>64</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="L48" s="1"/>
       <c r="M48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49"/>
+        <v>48</v>
+      </c>
       <c r="C49" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D49" t="s">
         <v>188</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F49" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G49" t="s">
-        <v>192</v>
-      </c>
-      <c r="H49" t="s">
-        <v>193</v>
-      </c>
-      <c r="I49"/>
+        <v>83</v>
+      </c>
       <c r="J49" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50"/>
+      <c r="C50" t="s">
+        <v>190</v>
+      </c>
+      <c r="D50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50" t="s">
+        <v>193</v>
+      </c>
+      <c r="I50"/>
+      <c r="J50" t="s">
+        <v>73</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L50" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M50" t="s">
         <v>75</v>
       </c>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-      <c r="S49"/>
-      <c r="T49"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-    </row>
-    <row r="50" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A50" s="11" t="s">
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+    </row>
+    <row r="51" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E51" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="12" t="s">
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="L51" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M50" s="11" t="s">
+      <c r="M51" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N50" s="11" t="s">
+      <c r="N51" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-    </row>
-    <row r="51" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+    </row>
+    <row r="52" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>166</v>
       </c>
-      <c r="B51"/>
-      <c r="C51" t="s">
+      <c r="B52"/>
+      <c r="C52" t="s">
         <v>198</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>188</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>166</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>71</v>
       </c>
-      <c r="G51"/>
-      <c r="H51" t="s">
+      <c r="G52"/>
+      <c r="H52" t="s">
         <v>166</v>
       </c>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51" s="1" t="s">
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L51" s="1"/>
-      <c r="M51" t="s">
+      <c r="L52" s="1"/>
+      <c r="M52" t="s">
         <v>34</v>
       </c>
-      <c r="N51"/>
-      <c r="O51"/>
-      <c r="P51"/>
-      <c r="Q51"/>
-      <c r="R51"/>
-      <c r="S51"/>
-      <c r="T51"/>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-    </row>
-    <row r="52" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M52" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N52" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+    </row>
+    <row r="53" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="11"/>
       <c r="C53" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J53" s="11"/>
+        <v>201</v>
+      </c>
       <c r="K53" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L53" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M53" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N53" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
-      <c r="V53" s="11"/>
-      <c r="W53" s="11"/>
-      <c r="X53" s="11"/>
-    </row>
-    <row r="54" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    </row>
+    <row r="54" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A54" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B54"/>
-      <c r="C54" t="s">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J54" s="11"/>
+      <c r="K54" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M54" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N54" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="11"/>
+      <c r="U54" s="11"/>
+      <c r="V54" s="11"/>
+      <c r="W54" s="11"/>
+      <c r="X54" s="11"/>
+    </row>
+    <row r="55" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55"/>
+      <c r="C55" t="s">
         <v>210</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>188</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>205</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
         <v>211</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>211</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>205</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>211</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>64</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M55" t="s">
         <v>54</v>
       </c>
-      <c r="N54"/>
-      <c r="O54"/>
-      <c r="P54"/>
-      <c r="Q54"/>
-      <c r="R54"/>
-      <c r="S54"/>
-      <c r="T54"/>
-      <c r="U54"/>
-      <c r="V54"/>
-      <c r="W54"/>
-      <c r="X54"/>
-    </row>
-    <row r="55" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+    </row>
+    <row r="56" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11" t="s">
+      <c r="B56" s="11"/>
+      <c r="C56" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F56" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G56" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="H56" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I55" s="11" t="s">
+      <c r="I56" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J55" s="11" t="s">
+      <c r="J56" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K55" s="12" t="s">
+      <c r="K56" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L55" s="12" t="s">
+      <c r="L56" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="11"/>
-      <c r="U55" s="11"/>
-      <c r="V55" s="11"/>
-      <c r="W55" s="11"/>
-      <c r="X55" s="11"/>
-    </row>
-    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+    </row>
+    <row r="57" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>19</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>218</v>
-      </c>
-      <c r="D56" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56" t="s">
-        <v>220</v>
-      </c>
-      <c r="G56" t="s">
-        <v>220</v>
-      </c>
-      <c r="H56" t="s">
-        <v>219</v>
-      </c>
-      <c r="I56" t="s">
-        <v>220</v>
-      </c>
-      <c r="J56" t="s">
-        <v>64</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M56" t="s">
-        <v>54</v>
-      </c>
-      <c r="N56" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>215</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
       </c>
       <c r="D57" t="s">
         <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F57" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G57" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H57" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I57" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J57" t="s">
         <v>64</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="N57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C58" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D58" t="s">
         <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F58" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G58" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H58" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I58" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J58" t="s">
         <v>64</v>
@@ -3391,30 +3413,24 @@
         <v>73</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M58" t="s">
-        <v>75</v>
-      </c>
-      <c r="N58" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>69</v>
       </c>
-      <c r="B59">
-        <v>34</v>
-      </c>
       <c r="C59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D59" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F59" t="s">
         <v>71</v>
@@ -3423,7 +3439,7 @@
         <v>71</v>
       </c>
       <c r="H59" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I59" t="s">
         <v>71</v>
@@ -3435,7 +3451,7 @@
         <v>73</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M59" t="s">
         <v>75</v>
@@ -3446,170 +3462,170 @@
     </row>
     <row r="60" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
       <c r="B60">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D60" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F60" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G60" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="H60" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I60" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="J60" t="s">
         <v>64</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M60" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="N60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B61">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D61" t="s">
         <v>188</v>
       </c>
       <c r="E61" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F61" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G61" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H61" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I61" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J61" t="s">
         <v>64</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M61" t="s">
         <v>56</v>
       </c>
       <c r="N61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>215</v>
+      </c>
+      <c r="B62">
+        <v>46</v>
+      </c>
+      <c r="C62" t="s">
+        <v>241</v>
+      </c>
+      <c r="D62" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" t="s">
+        <v>215</v>
+      </c>
+      <c r="F62" t="s">
+        <v>242</v>
+      </c>
+      <c r="G62" t="s">
+        <v>242</v>
+      </c>
+      <c r="H62" t="s">
+        <v>215</v>
+      </c>
+      <c r="I62" t="s">
+        <v>242</v>
+      </c>
+      <c r="J62" t="s">
+        <v>64</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M62" t="s">
+        <v>56</v>
+      </c>
+      <c r="N62" t="s">
         <v>244</v>
       </c>
-      <c r="O61"/>
-      <c r="P61"/>
-      <c r="Q61"/>
-      <c r="R61"/>
-      <c r="S61"/>
-      <c r="T61"/>
-      <c r="U61"/>
-      <c r="V61"/>
-      <c r="W61"/>
-      <c r="X61"/>
-    </row>
-    <row r="62" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A62" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="11">
-        <v>48</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J62" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K62" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L62" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M62" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N62" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62"/>
+    </row>
+    <row r="63" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J63" s="11" t="s">
         <v>64</v>
@@ -3618,131 +3634,134 @@
         <v>73</v>
       </c>
       <c r="L63" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M63" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N63" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
-      <c r="T63" s="11"/>
-      <c r="U63" s="11"/>
-      <c r="V63" s="11"/>
-      <c r="W63" s="11"/>
-      <c r="X63" s="11"/>
-    </row>
-    <row r="64" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    </row>
+    <row r="64" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A64" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B64">
-        <v>54</v>
-      </c>
-      <c r="C64" t="s">
-        <v>255</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="B64" s="11">
+        <v>49</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E64" t="s">
-        <v>258</v>
-      </c>
-      <c r="F64" t="s">
-        <v>257</v>
-      </c>
-      <c r="G64" t="s">
-        <v>257</v>
-      </c>
-      <c r="H64" t="s">
-        <v>256</v>
-      </c>
-      <c r="I64" t="s">
-        <v>257</v>
-      </c>
-      <c r="J64" t="s">
+      <c r="E64" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J64" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M64" t="s">
+      <c r="K64" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L64" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M64" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" ht="174" x14ac:dyDescent="0.35">
+      <c r="N64" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11"/>
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+    </row>
+    <row r="65" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>19</v>
       </c>
+      <c r="B65">
+        <v>54</v>
+      </c>
       <c r="C65" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D65" t="s">
         <v>188</v>
       </c>
       <c r="E65" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F65" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G65" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H65" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I65" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J65" t="s">
         <v>64</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M65" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>19</v>
       </c>
-      <c r="B66">
-        <v>80</v>
-      </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D66" t="s">
         <v>188</v>
       </c>
       <c r="E66" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F66" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G66" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H66" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I66" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J66" t="s">
         <v>64</v>
@@ -3750,38 +3769,37 @@
       <c r="K66" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L66" s="1"/>
+      <c r="L66" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M66" t="s">
         <v>264</v>
       </c>
-      <c r="N66" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>19</v>
       </c>
       <c r="B67">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C67" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D67" t="s">
         <v>188</v>
       </c>
       <c r="E67" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F67" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G67" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H67" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I67" t="s">
         <v>220</v>
@@ -3790,20 +3808,59 @@
         <v>64</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L67" s="1"/>
       <c r="M67" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N67" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L68" s="1"/>
+    <row r="68" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68">
+        <v>189</v>
+      </c>
+      <c r="C68" t="s">
+        <v>278</v>
+      </c>
+      <c r="D68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" t="s">
+        <v>279</v>
+      </c>
+      <c r="F68" t="s">
+        <v>280</v>
+      </c>
+      <c r="G68" t="s">
+        <v>83</v>
+      </c>
+      <c r="H68" t="s">
+        <v>281</v>
+      </c>
+      <c r="I68" t="s">
+        <v>220</v>
+      </c>
+      <c r="J68" t="s">
+        <v>64</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M68" t="s">
+        <v>114</v>
+      </c>
+      <c r="N68" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L69" s="1"/>
@@ -3834,6 +3891,9 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L78" s="1"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 35 python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5264EE88-21FC-4A82-9486-809B8CAEC036}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9F27AE-54ED-4020-AB23-CDE9C7B4579D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="318">
   <si>
     <t>Problem Type</t>
   </si>
@@ -973,6 +973,24 @@
   </si>
   <si>
     <t>1 hour 20 minutes</t>
+  </si>
+  <si>
+    <t>338-Counting Bits</t>
+  </si>
+  <si>
+    <t>Double loop with some hashtabe intelegence</t>
+  </si>
+  <si>
+    <t>O(nlongn) time, O(n) memory</t>
+  </si>
+  <si>
+    <t>Dynamic programing via most significat bit memoization</t>
+  </si>
+  <si>
+    <t>35-Search Insert Position</t>
+  </si>
+  <si>
+    <t>Binary Search Array</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1102,6 +1120,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1130,8 +1151,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X81" totalsRowShown="0">
-  <autoFilter ref="A2:X81" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X83" totalsRowShown="0">
+  <autoFilter ref="A2:X83" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1459,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X81"/>
+  <dimension ref="A2:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1811,153 +1832,152 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="K10"/>
+      <c r="L10" s="1"/>
+      <c r="M10" t="s">
+        <v>264</v>
+      </c>
+      <c r="N10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
         <v>67</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>68</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>69</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>70</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
         <v>69</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>71</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>72</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>169</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13">
-        <v>26</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
         <v>73</v>
       </c>
+      <c r="K13"/>
       <c r="L13" s="1"/>
-      <c r="M13" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s">
         <v>83</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
       </c>
       <c r="I14" t="s">
         <v>83</v>
@@ -1967,242 +1987,251 @@
       </c>
       <c r="L14" s="1"/>
       <c r="M14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15"/>
-      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>288</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>289</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
         <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="13"/>
+        <v>83</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="K16"/>
       <c r="L16" s="1"/>
-      <c r="M16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="3"/>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>288</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>289</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="H17" s="13"/>
       <c r="I17" t="s">
-        <v>46</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K17"/>
       <c r="L17" s="1"/>
       <c r="M17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>96</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>97</v>
       </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
         <v>98</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>99</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>99</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>99</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="M19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>91</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21">
         <v>112</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>302</v>
       </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
         <v>303</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>304</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>305</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>303</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>247</v>
       </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>109</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>108</v>
       </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
         <v>109</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>110</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>110</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>64</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" t="s">
-        <v>83</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M22" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -2210,13 +2239,13 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F23" t="s">
         <v>83</v>
@@ -2226,21 +2255,21 @@
       </c>
       <c r="L23" s="1"/>
       <c r="M23" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F24" t="s">
         <v>83</v>
@@ -2250,124 +2279,116 @@
       </c>
       <c r="L24" s="1"/>
       <c r="M24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I25" t="s">
         <v>83</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" t="s">
-        <v>124</v>
+      <c r="C26" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H26" t="s">
-        <v>125</v>
+        <v>83</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="I26" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="L26" s="1"/>
       <c r="M26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="H27" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="I27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" t="s">
+        <v>64</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F28" t="s">
         <v>83</v>
@@ -2375,352 +2396,360 @@
       <c r="G28" t="s">
         <v>83</v>
       </c>
-      <c r="I28" t="s">
-        <v>83</v>
+      <c r="H28" t="s">
+        <v>128</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M28" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" t="s">
+        <v>83</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F30" t="s">
         <v>72</v>
       </c>
-      <c r="G30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" t="s">
-        <v>72</v>
-      </c>
       <c r="K30" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="M30" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
         <v>143</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>144</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>71</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J32" t="s">
         <v>73</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" t="s">
-        <v>148</v>
-      </c>
-      <c r="I32" t="s">
-        <v>148</v>
-      </c>
-      <c r="J32" t="s">
-        <v>64</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L32" s="1"/>
+      <c r="L32" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="M32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="3"/>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F33" t="s">
-        <v>83</v>
+        <v>148</v>
+      </c>
+      <c r="G33" t="s">
+        <v>148</v>
+      </c>
+      <c r="I33" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34">
-        <v>226</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>293</v>
+        <v>150</v>
       </c>
       <c r="F34" t="s">
-        <v>294</v>
-      </c>
-      <c r="G34" t="s">
-        <v>294</v>
+        <v>83</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35">
+        <v>226</v>
+      </c>
+      <c r="C35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
+        <v>293</v>
+      </c>
+      <c r="F35" t="s">
+        <v>294</v>
+      </c>
+      <c r="G35" t="s">
+        <v>294</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>153</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>154</v>
       </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
         <v>155</v>
       </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="M36" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="6">
+        <v>338</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>157</v>
       </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
         <v>158</v>
       </c>
-      <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I36" t="s">
-        <v>83</v>
-      </c>
-      <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" t="s">
+        <v>83</v>
+      </c>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>159</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>160</v>
       </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>161</v>
       </c>
-      <c r="F37" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" t="s">
-        <v>83</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" t="s">
+        <v>83</v>
+      </c>
+      <c r="J39" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M39" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
-        <v>164</v>
-      </c>
-      <c r="F38" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" t="s">
-        <v>83</v>
-      </c>
-      <c r="H38" t="s">
-        <v>23</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="M38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" t="s">
-        <v>167</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" t="s">
-        <v>169</v>
-      </c>
-      <c r="G39" t="s">
-        <v>170</v>
-      </c>
-      <c r="H39" t="s">
-        <v>166</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D40" t="s">
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F40" t="s">
         <v>83</v>
@@ -2731,52 +2760,54 @@
       <c r="H40" t="s">
         <v>23</v>
       </c>
+      <c r="K40" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="L40" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="M40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>166</v>
+      </c>
       <c r="C41" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F41" t="s">
-        <v>176</v>
-      </c>
-      <c r="I41" t="s">
-        <v>178</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
+      </c>
+      <c r="G41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H41" t="s">
+        <v>166</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="M41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
         <v>83</v>
@@ -2784,208 +2815,212 @@
       <c r="G42" t="s">
         <v>83</v>
       </c>
-      <c r="I42" t="s">
-        <v>83</v>
-      </c>
-      <c r="J42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>64</v>
+      <c r="H42" t="s">
+        <v>23</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="M42" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B43">
-        <v>392</v>
-      </c>
+      <c r="B43" s="3"/>
       <c r="C43" t="s">
-        <v>290</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
       <c r="F43" t="s">
-        <v>83</v>
-      </c>
-      <c r="G43" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
       <c r="I43" t="s">
-        <v>83</v>
-      </c>
-      <c r="J43" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L43" s="1"/>
+      <c r="L43" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="M43" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
       </c>
-      <c r="L44" s="1"/>
+      <c r="G44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" t="s">
+        <v>64</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M44" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" s="10" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="10">
-        <v>572</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="M45" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45">
+        <v>392</v>
+      </c>
+      <c r="C45" t="s">
+        <v>290</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L45" s="1"/>
+      <c r="M45" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>19</v>
       </c>
+      <c r="B46"/>
       <c r="C46" t="s">
-        <v>265</v>
+        <v>184</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F46" t="s">
         <v>83</v>
       </c>
-      <c r="G46" t="s">
-        <v>83</v>
-      </c>
-      <c r="H46" t="s">
-        <v>266</v>
-      </c>
-      <c r="I46" t="s">
-        <v>83</v>
-      </c>
-      <c r="J46" t="s">
-        <v>267</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" t="s">
-        <v>268</v>
-      </c>
-      <c r="N46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+    </row>
+    <row r="47" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+      <c r="A47" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="10">
+        <v>572</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="M47" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>19</v>
       </c>
-      <c r="B47">
-        <v>58</v>
-      </c>
-      <c r="C47" t="s">
-        <v>270</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" t="s">
-        <v>271</v>
-      </c>
-      <c r="F47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G47" t="s">
-        <v>83</v>
-      </c>
-      <c r="H47" t="s">
-        <v>271</v>
-      </c>
-      <c r="I47" t="s">
-        <v>83</v>
-      </c>
-      <c r="J47" t="s">
-        <v>64</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L47" s="1"/>
-      <c r="M47" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48">
-        <v>205</v>
-      </c>
       <c r="C48" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="F48" t="s">
         <v>83</v>
@@ -2994,22 +3029,20 @@
         <v>83</v>
       </c>
       <c r="H48" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="I48" t="s">
         <v>83</v>
       </c>
       <c r="J48" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="L48" s="1"/>
       <c r="M48" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="N48" t="s">
         <v>105</v>
@@ -3020,54 +3053,66 @@
         <v>19</v>
       </c>
       <c r="B49">
-        <v>252</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="F49" t="s">
-        <v>285</v>
+        <v>83</v>
       </c>
       <c r="G49" t="s">
-        <v>286</v>
+        <v>83</v>
+      </c>
+      <c r="H49" t="s">
+        <v>271</v>
       </c>
       <c r="I49" t="s">
-        <v>287</v>
+        <v>83</v>
       </c>
       <c r="J49" t="s">
         <v>64</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>141</v>
+      </c>
+      <c r="B50">
+        <v>205</v>
       </c>
       <c r="C50" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
       <c r="D50" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
       <c r="F50" t="s">
         <v>83</v>
       </c>
       <c r="G50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" t="s">
+        <v>275</v>
+      </c>
+      <c r="I50" t="s">
         <v>83</v>
       </c>
       <c r="J50" t="s">
@@ -3077,479 +3122,442 @@
         <v>73</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>189</v>
+        <v>276</v>
       </c>
       <c r="M50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+      <c r="N50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>19</v>
       </c>
-      <c r="B51"/>
+      <c r="B51">
+        <v>252</v>
+      </c>
       <c r="C51" t="s">
+        <v>283</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>284</v>
+      </c>
+      <c r="F51" t="s">
+        <v>285</v>
+      </c>
+      <c r="G51" t="s">
+        <v>286</v>
+      </c>
+      <c r="I51" t="s">
+        <v>287</v>
+      </c>
+      <c r="J51" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L51" s="1"/>
+      <c r="M51" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52"/>
+      <c r="C52" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" t="s">
+        <v>161</v>
+      </c>
+      <c r="F52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G52" t="s">
+        <v>83</v>
+      </c>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M52" t="s">
+        <v>56</v>
+      </c>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+    </row>
+    <row r="53" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
         <v>190</v>
-      </c>
-      <c r="D51" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" t="s">
-        <v>60</v>
-      </c>
-      <c r="F51" t="s">
-        <v>191</v>
-      </c>
-      <c r="G51" t="s">
-        <v>192</v>
-      </c>
-      <c r="H51" t="s">
-        <v>193</v>
-      </c>
-      <c r="I51"/>
-      <c r="J51" t="s">
-        <v>73</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="M51" t="s">
-        <v>75</v>
-      </c>
-      <c r="N51"/>
-      <c r="O51"/>
-      <c r="P51"/>
-      <c r="Q51"/>
-      <c r="R51"/>
-      <c r="S51"/>
-      <c r="T51"/>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-    </row>
-    <row r="52" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="M52" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N52" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
-      <c r="X52" s="11"/>
-    </row>
-    <row r="53" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>166</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53" t="s">
-        <v>198</v>
       </c>
       <c r="D53" t="s">
         <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>166</v>
+        <v>60</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
-      </c>
-      <c r="G53"/>
+        <v>191</v>
+      </c>
+      <c r="G53" t="s">
+        <v>192</v>
+      </c>
       <c r="H53" t="s">
-        <v>166</v>
-      </c>
-      <c r="I53"/>
-      <c r="J53"/>
+        <v>193</v>
+      </c>
+      <c r="J53" t="s">
+        <v>73</v>
+      </c>
       <c r="K53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L53" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="M53" t="s">
-        <v>34</v>
-      </c>
-      <c r="N53"/>
-      <c r="O53"/>
-      <c r="P53"/>
-      <c r="Q53"/>
-      <c r="R53"/>
-      <c r="S53"/>
-      <c r="T53"/>
-      <c r="U53"/>
-      <c r="V53"/>
-      <c r="W53"/>
-      <c r="X53"/>
-    </row>
-    <row r="54" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" s="11" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="K54" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L54" s="12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="M54" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N54" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+    <row r="55" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55"/>
+      <c r="C55" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" t="s">
+        <v>166</v>
+      </c>
+      <c r="F55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55"/>
+      <c r="H55" t="s">
+        <v>166</v>
+      </c>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L55" s="1"/>
+      <c r="M55" t="s">
+        <v>34</v>
+      </c>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+    </row>
+    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A56" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11" t="s">
+      <c r="B56" s="11"/>
+      <c r="C56" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J56" s="11"/>
+      <c r="K56" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="M56" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N56" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+    </row>
+    <row r="57" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J55" s="11"/>
-      <c r="K55" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="M55" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="N55" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="11"/>
-      <c r="U55" s="11"/>
-      <c r="V55" s="11"/>
-      <c r="W55" s="11"/>
-      <c r="X55" s="11"/>
-    </row>
-    <row r="56" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56"/>
-      <c r="C56" t="s">
-        <v>210</v>
-      </c>
-      <c r="D56" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" t="s">
-        <v>205</v>
-      </c>
-      <c r="F56" t="s">
-        <v>211</v>
-      </c>
-      <c r="G56" t="s">
-        <v>211</v>
-      </c>
-      <c r="H56" t="s">
-        <v>205</v>
-      </c>
-      <c r="I56" t="s">
-        <v>211</v>
-      </c>
-      <c r="J56" t="s">
-        <v>64</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="M56" t="s">
-        <v>54</v>
-      </c>
-      <c r="N56"/>
-      <c r="O56"/>
-      <c r="P56"/>
-      <c r="Q56"/>
-      <c r="R56"/>
-      <c r="S56"/>
-      <c r="T56"/>
-      <c r="U56"/>
-      <c r="V56"/>
-      <c r="W56"/>
-      <c r="X56"/>
-    </row>
-    <row r="57" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
-      <c r="U57" s="11"/>
-      <c r="V57" s="11"/>
-      <c r="W57" s="11"/>
-      <c r="X57" s="11"/>
-    </row>
-    <row r="58" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N57" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D58" t="s">
         <v>188</v>
       </c>
       <c r="E58" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="F58" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G58" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H58" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="I58" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J58" t="s">
         <v>64</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="M58" t="s">
         <v>54</v>
       </c>
-      <c r="N58" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    </row>
+    <row r="59" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C59" t="s">
-        <v>223</v>
-      </c>
-      <c r="D59" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" t="s">
-        <v>224</v>
-      </c>
-      <c r="F59" t="s">
-        <v>225</v>
-      </c>
-      <c r="G59" t="s">
-        <v>225</v>
-      </c>
-      <c r="H59" t="s">
-        <v>224</v>
-      </c>
-      <c r="I59" t="s">
-        <v>225</v>
-      </c>
-      <c r="J59" t="s">
+      <c r="F59" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="M59" t="s">
-        <v>55</v>
-      </c>
+      <c r="K59" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
+      <c r="V59" s="11"/>
+      <c r="W59" s="11"/>
+      <c r="X59" s="11"/>
     </row>
     <row r="60" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D60" t="s">
         <v>188</v>
       </c>
       <c r="E60" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F60" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="G60" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="H60" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I60" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="J60" t="s">
         <v>64</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="M60" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="N60" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="C61" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D61" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E61" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F61" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G61" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H61" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="I61" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J61" t="s">
         <v>64</v>
@@ -3558,86 +3566,80 @@
         <v>73</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="M61" t="s">
-        <v>75</v>
-      </c>
-      <c r="N61" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>234</v>
-      </c>
-      <c r="B62">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F62" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="G62" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="H62" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="I62" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="J62" t="s">
         <v>64</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="M62" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="N62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="B63">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C63" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D63" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="E63" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="F63" t="s">
-        <v>242</v>
+        <v>71</v>
       </c>
       <c r="G63" t="s">
-        <v>242</v>
+        <v>71</v>
       </c>
       <c r="H63" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="I63" t="s">
-        <v>242</v>
+        <v>71</v>
       </c>
       <c r="J63" t="s">
         <v>64</v>
@@ -3646,309 +3648,332 @@
         <v>73</v>
       </c>
       <c r="L63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M63" t="s">
+        <v>75</v>
+      </c>
+      <c r="N63" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" t="s">
+        <v>236</v>
+      </c>
+      <c r="F64" t="s">
+        <v>237</v>
+      </c>
+      <c r="G64" t="s">
+        <v>237</v>
+      </c>
+      <c r="H64" t="s">
+        <v>238</v>
+      </c>
+      <c r="I64" t="s">
+        <v>239</v>
+      </c>
+      <c r="J64" t="s">
+        <v>64</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M64" t="s">
+        <v>56</v>
+      </c>
+      <c r="N64" t="s">
+        <v>64</v>
+      </c>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64"/>
+    </row>
+    <row r="65" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>215</v>
+      </c>
+      <c r="B65">
+        <v>46</v>
+      </c>
+      <c r="C65" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65" t="s">
+        <v>215</v>
+      </c>
+      <c r="F65" t="s">
+        <v>242</v>
+      </c>
+      <c r="G65" t="s">
+        <v>242</v>
+      </c>
+      <c r="H65" t="s">
+        <v>215</v>
+      </c>
+      <c r="I65" t="s">
+        <v>242</v>
+      </c>
+      <c r="J65" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M65" t="s">
         <v>56</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N65" t="s">
         <v>244</v>
       </c>
-      <c r="O63"/>
-      <c r="P63"/>
-      <c r="Q63"/>
-      <c r="R63"/>
-      <c r="S63"/>
-      <c r="T63"/>
-      <c r="U63"/>
-      <c r="V63"/>
-      <c r="W63"/>
-      <c r="X63"/>
-    </row>
-    <row r="64" spans="1:24" s="11" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A64" s="11" t="s">
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65"/>
+    </row>
+    <row r="66" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+      <c r="A66" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B66" s="11">
         <v>48</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C66" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D66" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E66" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F66" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="I64" s="11" t="s">
+      <c r="H66" s="11"/>
+      <c r="I66" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J64" s="11" t="s">
+      <c r="J66" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K64" s="12" t="s">
+      <c r="K66" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L64" s="12" t="s">
+      <c r="L66" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="M64" s="11" t="s">
+      <c r="M66" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N64" s="11" t="s">
+      <c r="N66" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:24" ht="174" x14ac:dyDescent="0.35">
-      <c r="A65" s="11" t="s">
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="11"/>
+      <c r="U66" s="11"/>
+      <c r="V66" s="11"/>
+      <c r="W66" s="11"/>
+      <c r="X66" s="11"/>
+    </row>
+    <row r="67" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="A67" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B67" s="11">
         <v>49</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C67" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D67" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F67" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G67" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="H65" s="11" t="s">
+      <c r="H67" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="I65" s="11" t="s">
+      <c r="I67" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="J65" s="11" t="s">
+      <c r="J67" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K65" s="12" t="s">
+      <c r="K67" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L65" s="12" t="s">
+      <c r="L67" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="M65" s="11" t="s">
+      <c r="M67" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="N65" s="11" t="s">
+      <c r="N67" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
-      <c r="T65" s="11"/>
-      <c r="U65" s="11"/>
-      <c r="V65" s="11"/>
-      <c r="W65" s="11"/>
-      <c r="X65" s="11"/>
-    </row>
-    <row r="66" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66">
-        <v>54</v>
-      </c>
-      <c r="C66" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" t="s">
-        <v>188</v>
-      </c>
-      <c r="E66" t="s">
-        <v>258</v>
-      </c>
-      <c r="F66" t="s">
-        <v>257</v>
-      </c>
-      <c r="G66" t="s">
-        <v>257</v>
-      </c>
-      <c r="H66" t="s">
-        <v>256</v>
-      </c>
-      <c r="I66" t="s">
-        <v>257</v>
-      </c>
-      <c r="J66" t="s">
-        <v>64</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" ht="174" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="C67" t="s">
-        <v>260</v>
-      </c>
-      <c r="D67" t="s">
-        <v>188</v>
-      </c>
-      <c r="E67" t="s">
-        <v>261</v>
-      </c>
-      <c r="F67" t="s">
-        <v>262</v>
-      </c>
-      <c r="G67" t="s">
-        <v>262</v>
-      </c>
-      <c r="H67" t="s">
-        <v>261</v>
-      </c>
-      <c r="I67" t="s">
-        <v>262</v>
-      </c>
-      <c r="J67" t="s">
-        <v>64</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="M67" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+      <c r="Q67" s="11"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="11"/>
+      <c r="T67" s="11"/>
+      <c r="U67" s="11"/>
+      <c r="V67" s="11"/>
+      <c r="W67" s="11"/>
+      <c r="X67" s="11"/>
+    </row>
+    <row r="68" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>19</v>
       </c>
       <c r="B68">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="D68" t="s">
         <v>188</v>
       </c>
       <c r="E68" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F68" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="G68" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="H68" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="I68" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="J68" t="s">
         <v>64</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L68" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>259</v>
+      </c>
       <c r="M68" t="s">
-        <v>264</v>
-      </c>
-      <c r="N68" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" ht="174" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>19</v>
       </c>
-      <c r="B69">
-        <v>128</v>
-      </c>
       <c r="C69" t="s">
-        <v>306</v>
+        <v>260</v>
       </c>
       <c r="D69" t="s">
         <v>188</v>
       </c>
-      <c r="E69" s="15" t="s">
-        <v>307</v>
+      <c r="E69" t="s">
+        <v>261</v>
       </c>
       <c r="F69" t="s">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="G69" t="s">
-        <v>308</v>
-      </c>
-      <c r="H69" s="15" t="s">
-        <v>307</v>
+        <v>262</v>
+      </c>
+      <c r="H69" t="s">
+        <v>261</v>
       </c>
       <c r="I69" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
       <c r="J69" t="s">
         <v>64</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>310</v>
+        <v>263</v>
       </c>
       <c r="M69" t="s">
-        <v>311</v>
-      </c>
-      <c r="N69" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>19</v>
       </c>
       <c r="B70">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D70" t="s">
         <v>188</v>
       </c>
       <c r="E70" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F70" t="s">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="G70" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="H70" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="I70" t="s">
         <v>220</v>
@@ -3957,23 +3982,103 @@
         <v>64</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>282</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L70" s="1"/>
       <c r="M70" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="N70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="L72" s="1"/>
+    <row r="71" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71">
+        <v>128</v>
+      </c>
+      <c r="C71" t="s">
+        <v>306</v>
+      </c>
+      <c r="D71" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="F71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" t="s">
+        <v>308</v>
+      </c>
+      <c r="H71" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="I71" t="s">
+        <v>309</v>
+      </c>
+      <c r="J71" t="s">
+        <v>64</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="M71" t="s">
+        <v>311</v>
+      </c>
+      <c r="N71" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72">
+        <v>189</v>
+      </c>
+      <c r="C72" t="s">
+        <v>278</v>
+      </c>
+      <c r="D72" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" t="s">
+        <v>279</v>
+      </c>
+      <c r="F72" t="s">
+        <v>280</v>
+      </c>
+      <c r="G72" t="s">
+        <v>83</v>
+      </c>
+      <c r="H72" t="s">
+        <v>281</v>
+      </c>
+      <c r="I72" t="s">
+        <v>220</v>
+      </c>
+      <c r="J72" t="s">
+        <v>64</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M72" t="s">
+        <v>114</v>
+      </c>
+      <c r="N72" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="L73" s="1"/>
@@ -4001,6 +4106,12 @@
     </row>
     <row r="81" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L81" s="1"/>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L82" s="1"/>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L83" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 228 python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9F27AE-54ED-4020-AB23-CDE9C7B4579D}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AB6D7EF-FD48-4785-BC59-16403B188751}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="323">
   <si>
     <t>Problem Type</t>
   </si>
@@ -991,13 +991,28 @@
   </si>
   <si>
     <t>Binary Search Array</t>
+  </si>
+  <si>
+    <t>Intervals</t>
+  </si>
+  <si>
+    <t>228-SummaryRanges</t>
+  </si>
+  <si>
+    <t>Linear scan with first number of range stored</t>
+  </si>
+  <si>
+    <t>O(n), O(1) time</t>
+  </si>
+  <si>
+    <t>Challenge I had was really the edge cases of the array. Took me longer then I wanted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1027,6 +1042,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1120,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1151,8 +1172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X83" totalsRowShown="0">
-  <autoFilter ref="A2:X83" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X84" totalsRowShown="0">
+  <autoFilter ref="A2:X84" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1480,18 +1501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X83"/>
+  <dimension ref="A2:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="37.453125" customWidth="1"/>
     <col min="3" max="3" width="52.7265625" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" customWidth="1"/>
-    <col min="5" max="5" width="45.81640625" customWidth="1"/>
+    <col min="5" max="5" width="61.36328125" customWidth="1"/>
     <col min="6" max="6" width="33.54296875" customWidth="1"/>
     <col min="7" max="7" width="35.26953125" customWidth="1"/>
     <col min="8" max="8" width="48.1796875" customWidth="1"/>
@@ -1507,7 +1528,7 @@
     <col min="18" max="29" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="29">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +1640,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1655,7 +1676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1688,7 +1709,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="43.5">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1723,7 +1744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1756,7 +1777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="43.5">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1791,7 +1812,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="72.5">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1832,7 +1853,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="17.5">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1854,7 +1875,7 @@
       <c r="G10" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="2"/>
       <c r="K10"/>
       <c r="L10" s="1"/>
       <c r="M10" t="s">
@@ -1864,7 +1885,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1888,7 +1909,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="29">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1923,7 +1944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="17.5">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1957,7 +1978,7 @@
       <c r="K13"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1990,7 +2011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2023,7 +2044,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="15.5">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -2051,7 +2072,7 @@
       <c r="K16"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.5">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -2080,7 +2101,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -2108,7 +2129,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="72.5">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2140,7 +2161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="29">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2172,7 +2193,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -2202,7 +2223,7 @@
       </c>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="43.5">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2234,7 +2255,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2258,7 +2279,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2282,7 +2303,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -2306,7 +2327,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15.5">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2339,7 +2360,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="87">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2377,7 +2398,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="29">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2409,7 +2430,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="43.5">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -2441,7 +2462,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="43.5">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -2467,7 +2488,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="58">
       <c r="A31" t="s">
         <v>117</v>
       </c>
@@ -2499,7 +2520,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="43.5">
       <c r="A32" t="s">
         <v>141</v>
       </c>
@@ -2537,7 +2558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24">
       <c r="A33" s="3" t="s">
         <v>48</v>
       </c>
@@ -2571,7 +2592,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2592,7 +2613,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -2609,7 +2630,7 @@
         <v>293</v>
       </c>
       <c r="F35" t="s">
-        <v>294</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
         <v>294</v>
@@ -2622,286 +2643,280 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="58">
       <c r="A36" t="s">
+        <v>318</v>
+      </c>
+      <c r="B36">
+        <v>228</v>
+      </c>
+      <c r="C36" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="F36" t="s">
+        <v>321</v>
+      </c>
+      <c r="G36" t="s">
+        <v>321</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="M36" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="72.5">
+      <c r="A37" t="s">
         <v>153</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>154</v>
       </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
         <v>155</v>
       </c>
-      <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>83</v>
-      </c>
-      <c r="L36" s="1" t="s">
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M37" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
+    <row r="38" spans="1:24" s="6" customFormat="1">
+      <c r="A38" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B38" s="6">
         <v>338</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="G38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="6" t="s">
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="6" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:24">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>157</v>
       </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>158</v>
       </c>
-      <c r="F38" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" t="s">
-        <v>83</v>
-      </c>
-      <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" t="s">
+        <v>83</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:24" ht="29">
+      <c r="A40" t="s">
         <v>159</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>160</v>
       </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
         <v>161</v>
       </c>
-      <c r="F39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I39" t="s">
-        <v>83</v>
-      </c>
-      <c r="J39" t="s">
-        <v>64</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L39" s="1" t="s">
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40" t="s">
+        <v>64</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M40" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:24" ht="58">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>163</v>
       </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
         <v>164</v>
       </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" t="s">
-        <v>83</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="F41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:24" ht="72.5">
+      <c r="A42" t="s">
         <v>166</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>167</v>
       </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
         <v>168</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>169</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>170</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>166</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:24" ht="29">
+      <c r="A43" t="s">
         <v>19</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>172</v>
       </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
         <v>173</v>
       </c>
-      <c r="F42" t="s">
-        <v>83</v>
-      </c>
-      <c r="G42" t="s">
-        <v>83</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="F43" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" t="s">
         <v>23</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+    <row r="44" spans="1:24" ht="72.5">
+      <c r="A44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" t="s">
         <v>175</v>
       </c>
-      <c r="D43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
         <v>30</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>176</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I44" t="s">
         <v>178</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L43" s="1" t="s">
+      <c r="K44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M44" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" t="s">
-        <v>180</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" t="s">
-        <v>181</v>
-      </c>
-      <c r="F44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G44" t="s">
-        <v>83</v>
-      </c>
-      <c r="I44" t="s">
-        <v>83</v>
-      </c>
-      <c r="J44" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="M44" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" ht="43.5">
       <c r="A45" t="s">
         <v>19</v>
       </c>
-      <c r="B45">
-        <v>392</v>
-      </c>
       <c r="C45" t="s">
-        <v>290</v>
+        <v>180</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F45" t="s">
         <v>83</v>
@@ -2918,151 +2933,147 @@
       <c r="K45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L45" s="1"/>
+      <c r="L45" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="M45" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
       <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B46"/>
+      <c r="B46">
+        <v>392</v>
+      </c>
       <c r="C46" t="s">
-        <v>184</v>
+        <v>290</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F46" t="s">
         <v>83</v>
       </c>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46" s="1"/>
+      <c r="G46" t="s">
+        <v>83</v>
+      </c>
+      <c r="I46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="L46" s="1"/>
       <c r="M46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" s="10" customFormat="1">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47"/>
+      <c r="C47" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>185</v>
+      </c>
+      <c r="F47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" t="s">
         <v>186</v>
       </c>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
-      <c r="U46"/>
-      <c r="V46"/>
-      <c r="W46"/>
-      <c r="X46"/>
-    </row>
-    <row r="47" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+    </row>
+    <row r="48" spans="1:24" ht="58">
+      <c r="A48" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B48" s="10">
         <v>572</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="10" t="s">
+      <c r="D48" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F48" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G48" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="H48" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I48" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="J47" s="10"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14" t="s">
+      <c r="J48" s="10"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="M47" s="10" t="s">
+      <c r="M48" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
-      <c r="T47" s="10"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
-      <c r="W47" s="10"/>
-      <c r="X47" s="10"/>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>265</v>
-      </c>
-      <c r="D48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" t="s">
-        <v>173</v>
-      </c>
-      <c r="F48" t="s">
-        <v>83</v>
-      </c>
-      <c r="G48" t="s">
-        <v>83</v>
-      </c>
-      <c r="H48" t="s">
-        <v>266</v>
-      </c>
-      <c r="I48" t="s">
-        <v>83</v>
-      </c>
-      <c r="J48" t="s">
-        <v>267</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L48" s="1"/>
-      <c r="M48" t="s">
-        <v>268</v>
-      </c>
-      <c r="N48" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="10"/>
+      <c r="W48" s="10"/>
+      <c r="X48" s="10"/>
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49" t="s">
         <v>19</v>
       </c>
-      <c r="B49">
-        <v>58</v>
-      </c>
       <c r="C49" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="F49" t="s">
         <v>83</v>
@@ -3071,37 +3082,40 @@
         <v>83</v>
       </c>
       <c r="H49" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I49" t="s">
         <v>83</v>
       </c>
       <c r="J49" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="N49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B50">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D50" t="s">
         <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F50" t="s">
         <v>83</v>
@@ -3110,7 +3124,7 @@
         <v>83</v>
       </c>
       <c r="H50" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I50" t="s">
         <v>83</v>
@@ -3121,481 +3135,482 @@
       <c r="K50" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="L50" s="1"/>
+      <c r="M50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="72.5">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51">
+        <v>205</v>
+      </c>
+      <c r="C51" t="s">
+        <v>274</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G51" t="s">
+        <v>83</v>
+      </c>
+      <c r="H51" t="s">
+        <v>275</v>
+      </c>
+      <c r="I51" t="s">
+        <v>83</v>
+      </c>
+      <c r="J51" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="M50" t="s">
-        <v>277</v>
-      </c>
-      <c r="N50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51">
-        <v>252</v>
-      </c>
-      <c r="C51" t="s">
-        <v>283</v>
-      </c>
-      <c r="D51" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" t="s">
-        <v>284</v>
-      </c>
-      <c r="F51" t="s">
-        <v>285</v>
-      </c>
-      <c r="G51" t="s">
-        <v>286</v>
-      </c>
-      <c r="I51" t="s">
-        <v>287</v>
-      </c>
-      <c r="J51" t="s">
-        <v>64</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L51" s="1"/>
       <c r="M51" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="52" spans="1:24" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="N51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52">
+        <v>252</v>
+      </c>
+      <c r="C52" t="s">
+        <v>283</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>284</v>
+      </c>
+      <c r="F52" t="s">
+        <v>285</v>
+      </c>
+      <c r="G52" t="s">
+        <v>286</v>
+      </c>
+      <c r="I52" t="s">
+        <v>287</v>
+      </c>
+      <c r="J52" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L52" s="1"/>
+      <c r="M52" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="11" customFormat="1" ht="29">
+      <c r="A53" t="s">
         <v>48</v>
       </c>
-      <c r="B52"/>
-      <c r="C52" t="s">
+      <c r="B53"/>
+      <c r="C53" t="s">
         <v>187</v>
-      </c>
-      <c r="D52" t="s">
-        <v>188</v>
-      </c>
-      <c r="E52" t="s">
-        <v>161</v>
-      </c>
-      <c r="F52" t="s">
-        <v>83</v>
-      </c>
-      <c r="G52" t="s">
-        <v>83</v>
-      </c>
-      <c r="H52"/>
-      <c r="I52"/>
-      <c r="J52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M52" t="s">
-        <v>56</v>
-      </c>
-      <c r="N52"/>
-      <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
-      <c r="S52"/>
-      <c r="T52"/>
-      <c r="U52"/>
-      <c r="V52"/>
-      <c r="W52"/>
-      <c r="X52"/>
-    </row>
-    <row r="53" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>190</v>
       </c>
       <c r="D53" t="s">
         <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F53" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="G53" t="s">
-        <v>192</v>
-      </c>
-      <c r="H53" t="s">
-        <v>193</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="H53"/>
+      <c r="I53"/>
       <c r="J53" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M53" t="s">
+        <v>56</v>
+      </c>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+      <c r="V53"/>
+      <c r="W53"/>
+      <c r="X53"/>
+    </row>
+    <row r="54" spans="1:24" ht="58">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" t="s">
+        <v>191</v>
+      </c>
+      <c r="G54" t="s">
+        <v>192</v>
+      </c>
+      <c r="H54" t="s">
+        <v>193</v>
+      </c>
+      <c r="J54" t="s">
+        <v>73</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M54" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:24" s="11" customFormat="1" ht="145" x14ac:dyDescent="0.35">
-      <c r="A54" s="11" t="s">
+    <row r="55" spans="1:24" s="11" customFormat="1" ht="145">
+      <c r="A55" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C55" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K54" s="12" t="s">
+      <c r="K55" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L54" s="12" t="s">
+      <c r="L55" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="M54" s="11" t="s">
+      <c r="M55" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="N54" s="11" t="s">
+      <c r="N55" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:24" s="11" customFormat="1">
+      <c r="A56" t="s">
         <v>166</v>
       </c>
-      <c r="B55"/>
-      <c r="C55" t="s">
+      <c r="B56"/>
+      <c r="C56" t="s">
         <v>198</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>188</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>166</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
         <v>71</v>
       </c>
-      <c r="G55"/>
-      <c r="H55" t="s">
+      <c r="G56"/>
+      <c r="H56" t="s">
         <v>166</v>
       </c>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="K55" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L55" s="1"/>
-      <c r="M55" t="s">
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L56" s="1"/>
+      <c r="M56" t="s">
         <v>34</v>
       </c>
-      <c r="N55"/>
-      <c r="O55"/>
-      <c r="P55"/>
-      <c r="Q55"/>
-      <c r="R55"/>
-      <c r="S55"/>
-      <c r="T55"/>
-      <c r="U55"/>
-      <c r="V55"/>
-      <c r="W55"/>
-      <c r="X55"/>
-    </row>
-    <row r="56" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A56" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J56" s="11"/>
-      <c r="K56" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M56" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="N56" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
-      <c r="U56" s="11"/>
-      <c r="V56" s="11"/>
-      <c r="W56" s="11"/>
-      <c r="X56" s="11"/>
-    </row>
-    <row r="57" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+      <c r="U56"/>
+      <c r="V56"/>
+      <c r="W56"/>
+      <c r="X56"/>
+    </row>
+    <row r="57" spans="1:24" ht="87">
       <c r="A57" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="B57" s="11"/>
       <c r="C57" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>206</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="J57" s="11"/>
       <c r="K57" s="12" t="s">
         <v>73</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M57" s="11" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N57" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="58" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="11"/>
+      <c r="V57" s="11"/>
+      <c r="W57" s="11"/>
+      <c r="X57" s="11"/>
+    </row>
+    <row r="58" spans="1:24" s="11" customFormat="1" ht="116">
+      <c r="A58" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M58" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N58" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="130.5">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" t="s">
         <v>210</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>188</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>205</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>211</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>211</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H59" t="s">
         <v>205</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I59" t="s">
         <v>211</v>
       </c>
-      <c r="J58" t="s">
-        <v>64</v>
-      </c>
-      <c r="K58" s="1" t="s">
+      <c r="J59" t="s">
+        <v>64</v>
+      </c>
+      <c r="K59" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="11" t="s">
+    <row r="60" spans="1:24" ht="101.5">
+      <c r="A60" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11" t="s">
+      <c r="B60" s="11"/>
+      <c r="C60" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E60" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G60" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="H60" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="I60" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J59" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K59" s="12" t="s">
+      <c r="J60" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K60" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="L59" s="12" t="s">
+      <c r="L60" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
-      <c r="T59" s="11"/>
-      <c r="U59" s="11"/>
-      <c r="V59" s="11"/>
-      <c r="W59" s="11"/>
-      <c r="X59" s="11"/>
-    </row>
-    <row r="60" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+    </row>
+    <row r="61" spans="1:24" ht="87">
+      <c r="A61" t="s">
         <v>19</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>218</v>
-      </c>
-      <c r="D60" t="s">
-        <v>188</v>
-      </c>
-      <c r="E60" t="s">
-        <v>219</v>
-      </c>
-      <c r="F60" t="s">
-        <v>220</v>
-      </c>
-      <c r="G60" t="s">
-        <v>220</v>
-      </c>
-      <c r="H60" t="s">
-        <v>219</v>
-      </c>
-      <c r="I60" t="s">
-        <v>220</v>
-      </c>
-      <c r="J60" t="s">
-        <v>64</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="M60" t="s">
-        <v>54</v>
-      </c>
-      <c r="N60" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>215</v>
-      </c>
-      <c r="C61" t="s">
-        <v>223</v>
       </c>
       <c r="D61" t="s">
         <v>188</v>
       </c>
       <c r="E61" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F61" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G61" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H61" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I61" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J61" t="s">
         <v>64</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="N61" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" ht="72.5">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="C62" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
       </c>
       <c r="E62" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F62" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="G62" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="H62" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I62" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="J62" t="s">
         <v>64</v>
@@ -3604,30 +3619,24 @@
         <v>73</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M62" t="s">
-        <v>75</v>
-      </c>
-      <c r="N62" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" ht="130.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" ht="87">
       <c r="A63" t="s">
         <v>69</v>
       </c>
-      <c r="B63">
-        <v>34</v>
-      </c>
       <c r="C63" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D63" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="E63" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F63" t="s">
         <v>71</v>
@@ -3636,7 +3645,7 @@
         <v>71</v>
       </c>
       <c r="H63" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I63" t="s">
         <v>71</v>
@@ -3648,7 +3657,7 @@
         <v>73</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M63" t="s">
         <v>75</v>
@@ -3657,102 +3666,92 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:24" s="11" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:24" ht="130.5">
       <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64">
+        <v>34</v>
+      </c>
+      <c r="C64" t="s">
+        <v>230</v>
+      </c>
+      <c r="D64" t="s">
+        <v>231</v>
+      </c>
+      <c r="E64" t="s">
+        <v>232</v>
+      </c>
+      <c r="F64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G64" t="s">
+        <v>71</v>
+      </c>
+      <c r="H64" t="s">
+        <v>232</v>
+      </c>
+      <c r="I64" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" t="s">
+        <v>64</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M64" t="s">
+        <v>75</v>
+      </c>
+      <c r="N64" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" s="11" customFormat="1" ht="130.5">
+      <c r="A65" t="s">
         <v>234</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>36</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>235</v>
-      </c>
-      <c r="D64" t="s">
-        <v>188</v>
-      </c>
-      <c r="E64" t="s">
-        <v>236</v>
-      </c>
-      <c r="F64" t="s">
-        <v>237</v>
-      </c>
-      <c r="G64" t="s">
-        <v>237</v>
-      </c>
-      <c r="H64" t="s">
-        <v>238</v>
-      </c>
-      <c r="I64" t="s">
-        <v>239</v>
-      </c>
-      <c r="J64" t="s">
-        <v>64</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M64" t="s">
-        <v>56</v>
-      </c>
-      <c r="N64" t="s">
-        <v>64</v>
-      </c>
-      <c r="O64"/>
-      <c r="P64"/>
-      <c r="Q64"/>
-      <c r="R64"/>
-      <c r="S64"/>
-      <c r="T64"/>
-      <c r="U64"/>
-      <c r="V64"/>
-      <c r="W64"/>
-      <c r="X64"/>
-    </row>
-    <row r="65" spans="1:24" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>215</v>
-      </c>
-      <c r="B65">
-        <v>46</v>
-      </c>
-      <c r="C65" t="s">
-        <v>241</v>
       </c>
       <c r="D65" t="s">
         <v>188</v>
       </c>
       <c r="E65" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="F65" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G65" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H65" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="I65" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="J65" t="s">
         <v>64</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M65" t="s">
         <v>56</v>
       </c>
       <c r="N65" t="s">
-        <v>244</v>
+        <v>64</v>
       </c>
       <c r="O65"/>
       <c r="P65"/>
@@ -3765,85 +3764,85 @@
       <c r="W65"/>
       <c r="X65"/>
     </row>
-    <row r="66" spans="1:24" ht="87" x14ac:dyDescent="0.35">
-      <c r="A66" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="11">
-        <v>48</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D66" s="11" t="s">
+    <row r="66" spans="1:24" s="11" customFormat="1" ht="116">
+      <c r="A66" t="s">
+        <v>215</v>
+      </c>
+      <c r="B66">
+        <v>46</v>
+      </c>
+      <c r="C66" t="s">
+        <v>241</v>
+      </c>
+      <c r="D66" t="s">
         <v>188</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J66" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K66" s="12" t="s">
+      <c r="E66" t="s">
+        <v>215</v>
+      </c>
+      <c r="F66" t="s">
+        <v>242</v>
+      </c>
+      <c r="G66" t="s">
+        <v>242</v>
+      </c>
+      <c r="H66" t="s">
+        <v>215</v>
+      </c>
+      <c r="I66" t="s">
+        <v>242</v>
+      </c>
+      <c r="J66" t="s">
+        <v>64</v>
+      </c>
+      <c r="K66" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L66" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="M66" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="N66" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
-      <c r="U66" s="11"/>
-      <c r="V66" s="11"/>
-      <c r="W66" s="11"/>
-      <c r="X66" s="11"/>
-    </row>
-    <row r="67" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="L66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M66" t="s">
+        <v>56</v>
+      </c>
+      <c r="N66" t="s">
+        <v>244</v>
+      </c>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+    </row>
+    <row r="67" spans="1:24" ht="87">
       <c r="A67" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>188</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>253</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H67" s="11"/>
       <c r="I67" s="11" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J67" s="11" t="s">
         <v>64</v>
@@ -3852,10 +3851,10 @@
         <v>73</v>
       </c>
       <c r="L67" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M67" s="11" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="N67" s="11" t="s">
         <v>73</v>
@@ -3871,112 +3870,125 @@
       <c r="W67" s="11"/>
       <c r="X67" s="11"/>
     </row>
-    <row r="68" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="68" spans="1:24" ht="174">
+      <c r="A68" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B68">
-        <v>54</v>
-      </c>
-      <c r="C68" t="s">
-        <v>255</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="B68" s="11">
+        <v>49</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E68" t="s">
-        <v>258</v>
-      </c>
-      <c r="F68" t="s">
-        <v>257</v>
-      </c>
-      <c r="G68" t="s">
-        <v>257</v>
-      </c>
-      <c r="H68" t="s">
-        <v>256</v>
-      </c>
-      <c r="I68" t="s">
-        <v>257</v>
-      </c>
-      <c r="J68" t="s">
-        <v>64</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M68" t="s">
+      <c r="E68" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J68" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K68" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L68" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="M68" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" ht="174" x14ac:dyDescent="0.35">
+      <c r="N68" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+      <c r="Q68" s="11"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="11"/>
+      <c r="T68" s="11"/>
+      <c r="U68" s="11"/>
+      <c r="V68" s="11"/>
+      <c r="W68" s="11"/>
+      <c r="X68" s="11"/>
+    </row>
+    <row r="69" spans="1:24" ht="116">
       <c r="A69" t="s">
         <v>19</v>
       </c>
+      <c r="B69">
+        <v>54</v>
+      </c>
       <c r="C69" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D69" t="s">
         <v>188</v>
       </c>
       <c r="E69" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F69" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G69" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H69" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I69" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J69" t="s">
         <v>64</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M69" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="174">
       <c r="A70" t="s">
         <v>19</v>
       </c>
-      <c r="B70">
-        <v>80</v>
-      </c>
       <c r="C70" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D70" t="s">
         <v>188</v>
       </c>
       <c r="E70" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F70" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="G70" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="H70" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="I70" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J70" t="s">
         <v>64</v>
@@ -3984,134 +3996,175 @@
       <c r="K70" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L70" s="1"/>
+      <c r="L70" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="M70" t="s">
         <v>264</v>
       </c>
-      <c r="N70" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:24">
       <c r="A71" t="s">
         <v>19</v>
       </c>
       <c r="B71">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="C71" t="s">
-        <v>306</v>
+        <v>272</v>
       </c>
       <c r="D71" t="s">
         <v>188</v>
       </c>
-      <c r="E71" s="15" t="s">
-        <v>307</v>
+      <c r="E71" t="s">
+        <v>273</v>
       </c>
       <c r="F71" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="G71" t="s">
-        <v>308</v>
-      </c>
-      <c r="H71" s="15" t="s">
-        <v>307</v>
+        <v>220</v>
+      </c>
+      <c r="H71" t="s">
+        <v>220</v>
       </c>
       <c r="I71" t="s">
-        <v>309</v>
+        <v>220</v>
       </c>
       <c r="J71" t="s">
         <v>64</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>310</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L71" s="1"/>
       <c r="M71" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="N71" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="145">
       <c r="A72" t="s">
         <v>19</v>
       </c>
       <c r="B72">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="C72" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="D72" t="s">
         <v>188</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="F72" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72" t="s">
+        <v>308</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="I72" t="s">
+        <v>309</v>
+      </c>
+      <c r="J72" t="s">
+        <v>64</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="M72" t="s">
+        <v>311</v>
+      </c>
+      <c r="N72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" ht="203">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73">
+        <v>189</v>
+      </c>
+      <c r="C73" t="s">
+        <v>278</v>
+      </c>
+      <c r="D73" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" t="s">
         <v>279</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F73" t="s">
         <v>280</v>
       </c>
-      <c r="G72" t="s">
-        <v>83</v>
-      </c>
-      <c r="H72" t="s">
+      <c r="G73" t="s">
+        <v>83</v>
+      </c>
+      <c r="H73" t="s">
         <v>281</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I73" t="s">
         <v>220</v>
       </c>
-      <c r="J72" t="s">
-        <v>64</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L72" s="1" t="s">
+      <c r="J73" t="s">
+        <v>64</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="M72" t="s">
+      <c r="M73" t="s">
         <v>114</v>
       </c>
-      <c r="N72" t="s">
+      <c r="N73" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24">
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:24">
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:24">
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24">
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24">
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24">
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24">
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="12:12">
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="12:12">
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="12:12">
       <c r="L83" s="1"/>
+    </row>
+    <row r="84" spans="12:12">
+      <c r="L84" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 347 in python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AB6D7EF-FD48-4785-BC59-16403B188751}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD909525-0ACC-407D-BC6E-5D1FFF8500E7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="328">
   <si>
     <t>Problem Type</t>
   </si>
@@ -1006,6 +1006,21 @@
   </si>
   <si>
     <t>Challenge I had was really the edge cases of the array. Took me longer then I wanted</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>347-Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Heap with frequency counter</t>
+  </si>
+  <si>
+    <t>Quick sort</t>
+  </si>
+  <si>
+    <t>Had to study the heap data structure and then solved this one</t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
   <dimension ref="A2:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4133,8 +4148,43 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
-      <c r="L74" s="1"/>
+    <row r="74" spans="1:24" ht="43.5">
+      <c r="A74" t="s">
+        <v>323</v>
+      </c>
+      <c r="B74">
+        <v>347</v>
+      </c>
+      <c r="C74" t="s">
+        <v>324</v>
+      </c>
+      <c r="D74" t="s">
+        <v>188</v>
+      </c>
+      <c r="E74" t="s">
+        <v>325</v>
+      </c>
+      <c r="F74" t="s">
+        <v>285</v>
+      </c>
+      <c r="H74" t="s">
+        <v>326</v>
+      </c>
+      <c r="J74" t="s">
+        <v>64</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M74" t="s">
+        <v>101</v>
+      </c>
+      <c r="N74" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="75" spans="1:24">
       <c r="L75" s="1"/>

</xml_diff>

<commit_message>
Solved problem 271 in python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD909525-0ACC-407D-BC6E-5D1FFF8500E7}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA45CD92-75DB-4055-9922-9C5600ACB787}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="331">
   <si>
     <t>Problem Type</t>
   </si>
@@ -1021,6 +1021,15 @@
   </si>
   <si>
     <t>Had to study the heap data structure and then solved this one</t>
+  </si>
+  <si>
+    <t>271 - Encode and Decode Strings</t>
+  </si>
+  <si>
+    <t>Build string with a number + delimiter denoting the next array element</t>
+  </si>
+  <si>
+    <t>Decoding the string was tricky to write the python code and manipulate the string positions</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
   <dimension ref="A2:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4186,8 +4195,49 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
-      <c r="L75" s="1"/>
+    <row r="75" spans="1:24" ht="72.5">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75">
+        <v>271</v>
+      </c>
+      <c r="C75" t="s">
+        <v>328</v>
+      </c>
+      <c r="D75" t="s">
+        <v>188</v>
+      </c>
+      <c r="E75" t="s">
+        <v>329</v>
+      </c>
+      <c r="F75" t="s">
+        <v>192</v>
+      </c>
+      <c r="G75" t="s">
+        <v>192</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="I75" t="s">
+        <v>192</v>
+      </c>
+      <c r="J75" t="s">
+        <v>64</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M75" t="s">
+        <v>75</v>
+      </c>
+      <c r="N75" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="76" spans="1:24">
       <c r="L76" s="1"/>

</xml_diff>

<commit_message>
Solved problem 238 in python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA45CD92-75DB-4055-9922-9C5600ACB787}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4109CBC3-0D51-4E7F-80C3-FB5EC8E18206}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="336">
   <si>
     <t>Problem Type</t>
   </si>
@@ -1030,6 +1030,21 @@
   </si>
   <si>
     <t>Decoding the string was tricky to write the python code and manipulate the string positions</t>
+  </si>
+  <si>
+    <t>238-Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Store left product and right product arrays to allow solution to be computed in linear time</t>
+  </si>
+  <si>
+    <t>Store left product and right product arrays within the input and output arrays</t>
+  </si>
+  <si>
+    <t>O(1) memory</t>
+  </si>
+  <si>
+    <t>2 hours 30 minutes</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1211,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X84" totalsRowShown="0">
-  <autoFilter ref="A2:X84" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X85" totalsRowShown="0">
+  <autoFilter ref="A2:X85" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1525,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X84"/>
+  <dimension ref="A2:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4157,71 +4172,69 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="43.5">
+    <row r="74" spans="1:24" ht="29">
       <c r="A74" t="s">
-        <v>323</v>
+        <v>19</v>
       </c>
       <c r="B74">
-        <v>347</v>
+        <v>238</v>
       </c>
       <c r="C74" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="D74" t="s">
         <v>188</v>
       </c>
-      <c r="E74" t="s">
-        <v>325</v>
+      <c r="E74" s="15" t="s">
+        <v>332</v>
       </c>
       <c r="F74" t="s">
-        <v>285</v>
-      </c>
-      <c r="H74" t="s">
-        <v>326</v>
+        <v>46</v>
+      </c>
+      <c r="G74" t="s">
+        <v>83</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="I74" t="s">
+        <v>334</v>
       </c>
       <c r="J74" t="s">
         <v>64</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>327</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L74" s="1"/>
       <c r="M74" t="s">
-        <v>101</v>
+        <v>335</v>
       </c>
       <c r="N74" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" ht="72.5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" ht="43.5">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>323</v>
       </c>
       <c r="B75">
-        <v>271</v>
+        <v>347</v>
       </c>
       <c r="C75" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D75" t="s">
         <v>188</v>
       </c>
       <c r="E75" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F75" t="s">
-        <v>192</v>
-      </c>
-      <c r="G75" t="s">
-        <v>192</v>
-      </c>
-      <c r="H75" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="I75" t="s">
-        <v>192</v>
+        <v>285</v>
+      </c>
+      <c r="H75" t="s">
+        <v>326</v>
       </c>
       <c r="J75" t="s">
         <v>64</v>
@@ -4230,17 +4243,58 @@
         <v>64</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M75" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="N75" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
-      <c r="L76" s="1"/>
+    <row r="76" spans="1:24" ht="72.5">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76">
+        <v>271</v>
+      </c>
+      <c r="C76" t="s">
+        <v>328</v>
+      </c>
+      <c r="D76" t="s">
+        <v>188</v>
+      </c>
+      <c r="E76" t="s">
+        <v>329</v>
+      </c>
+      <c r="F76" t="s">
+        <v>192</v>
+      </c>
+      <c r="G76" t="s">
+        <v>192</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="I76" t="s">
+        <v>192</v>
+      </c>
+      <c r="J76" t="s">
+        <v>64</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M76" t="s">
+        <v>75</v>
+      </c>
+      <c r="N76" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="77" spans="1:24">
       <c r="L77" s="1"/>
@@ -4265,6 +4319,9 @@
     </row>
     <row r="84" spans="12:12">
       <c r="L84" s="1"/>
+    </row>
+    <row r="85" spans="12:12">
+      <c r="L85" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved problem 155 in python
</commit_message>
<xml_diff>
--- a/LeetCodeList.xlsx
+++ b/LeetCodeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harriscomputer-my.sharepoint.com/personal/nserrano_harriscomputer_com/Documents/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4109CBC3-0D51-4E7F-80C3-FB5EC8E18206}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="13_ncr:1_{32E9F689-CACE-484E-90F6-D874180CB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E17E434D-39D9-4611-AE8A-54614E8393C4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F10354-735F-493B-9AA3-B7DCD10BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="346">
   <si>
     <t>Problem Type</t>
   </si>
@@ -1045,6 +1045,36 @@
   </si>
   <si>
     <t>2 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>155-Min Stack</t>
+  </si>
+  <si>
+    <t>Two stacks, one is the actual stack, the other used to track min values</t>
+  </si>
+  <si>
+    <t>O(1) time, O(n) memory</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>When I submitted my code, I missed one edge case where the same element could be pushed multiple times. I had to make sure the new minimums were also added to the second stack</t>
+  </si>
+  <si>
+    <t>150-Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>One pass scan using a stack</t>
+  </si>
+  <si>
+    <t>739-Daily Temperature</t>
+  </si>
+  <si>
+    <t>Linear scan utilizing stack</t>
+  </si>
+  <si>
+    <t>Linear scan utilizing stack with the array in place</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X85" totalsRowShown="0">
-  <autoFilter ref="A2:X85" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}" name="Table1" displayName="Table1" ref="A2:X87" totalsRowShown="0">
+  <autoFilter ref="A2:X87" xr:uid="{65FB70E7-0E2E-4490-95B0-13C0F68E3E86}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{32ABEBCD-9E91-4F42-978C-96FC4D58218D}" name="Problem Type"/>
     <tableColumn id="24" xr3:uid="{783B29D8-204A-49FE-93D6-CEA49D70CB6E}" name="Problem Number"/>
@@ -1540,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7E9D5C-2959-4E26-9C9F-C396742D2187}">
-  <dimension ref="A2:X85"/>
+  <dimension ref="A2:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4128,33 +4158,33 @@
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="203">
+    <row r="73" spans="1:24">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B73">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C73" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="D73" t="s">
         <v>188</v>
       </c>
-      <c r="E73" t="s">
-        <v>279</v>
+      <c r="E73" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="F73" t="s">
-        <v>280</v>
+        <v>46</v>
       </c>
       <c r="G73" t="s">
-        <v>83</v>
-      </c>
-      <c r="H73" t="s">
-        <v>281</v>
+        <v>46</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="I73" t="s">
-        <v>220</v>
+        <v>46</v>
       </c>
       <c r="J73" t="s">
         <v>64</v>
@@ -4162,79 +4192,79 @@
       <c r="K73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>282</v>
-      </c>
+      <c r="L73" s="1"/>
       <c r="M73" t="s">
-        <v>114</v>
-      </c>
-      <c r="N73" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" ht="29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" ht="130.5">
       <c r="A74" t="s">
         <v>19</v>
       </c>
       <c r="B74">
-        <v>238</v>
+        <v>155</v>
       </c>
       <c r="C74" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="D74" t="s">
         <v>188</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="F74" t="s">
-        <v>46</v>
+        <v>338</v>
       </c>
       <c r="G74" t="s">
-        <v>83</v>
+        <v>338</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="I74" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="J74" t="s">
         <v>64</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L74" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="M74" t="s">
-        <v>335</v>
-      </c>
-      <c r="N74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" ht="43.5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" ht="203">
       <c r="A75" t="s">
-        <v>323</v>
+        <v>19</v>
       </c>
       <c r="B75">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="C75" t="s">
-        <v>324</v>
+        <v>278</v>
       </c>
       <c r="D75" t="s">
         <v>188</v>
       </c>
       <c r="E75" t="s">
-        <v>325</v>
+        <v>279</v>
       </c>
       <c r="F75" t="s">
-        <v>285</v>
+        <v>280</v>
+      </c>
+      <c r="G75" t="s">
+        <v>83</v>
       </c>
       <c r="H75" t="s">
-        <v>326</v>
+        <v>281</v>
+      </c>
+      <c r="I75" t="s">
+        <v>220</v>
       </c>
       <c r="J75" t="s">
         <v>64</v>
@@ -4243,67 +4273,174 @@
         <v>64</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>327</v>
+        <v>282</v>
       </c>
       <c r="M75" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="N75" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" ht="72.5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" ht="29">
       <c r="A76" t="s">
         <v>19</v>
       </c>
       <c r="B76">
-        <v>271</v>
+        <v>238</v>
       </c>
       <c r="C76" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D76" t="s">
         <v>188</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="F76" t="s">
+        <v>46</v>
+      </c>
+      <c r="G76" t="s">
+        <v>83</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="I76" t="s">
+        <v>334</v>
+      </c>
+      <c r="J76" t="s">
+        <v>64</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L76" s="1"/>
+      <c r="M76" t="s">
+        <v>335</v>
+      </c>
+      <c r="N76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" ht="43.5">
+      <c r="A77" t="s">
+        <v>323</v>
+      </c>
+      <c r="B77">
+        <v>347</v>
+      </c>
+      <c r="C77" t="s">
+        <v>324</v>
+      </c>
+      <c r="D77" t="s">
+        <v>188</v>
+      </c>
+      <c r="E77" t="s">
+        <v>325</v>
+      </c>
+      <c r="F77" t="s">
+        <v>285</v>
+      </c>
+      <c r="H77" t="s">
+        <v>326</v>
+      </c>
+      <c r="J77" t="s">
+        <v>64</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M77" t="s">
+        <v>101</v>
+      </c>
+      <c r="N77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" ht="72.5">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78">
+        <v>271</v>
+      </c>
+      <c r="C78" t="s">
+        <v>328</v>
+      </c>
+      <c r="D78" t="s">
+        <v>188</v>
+      </c>
+      <c r="E78" t="s">
         <v>329</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F78" t="s">
         <v>192</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G78" t="s">
         <v>192</v>
       </c>
-      <c r="H76" s="15" t="s">
+      <c r="H78" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I78" t="s">
         <v>192</v>
       </c>
-      <c r="J76" t="s">
-        <v>64</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L76" s="1" t="s">
+      <c r="J78" t="s">
+        <v>64</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L78" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="M76" t="s">
+      <c r="M78" t="s">
         <v>75</v>
       </c>
-      <c r="N76" t="s">
+      <c r="N78" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:24">
-      <c r="L78" s="1"/>
-    </row>
     <row r="79" spans="1:24">
+      <c r="A79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79">
+        <v>739</v>
+      </c>
+      <c r="C79" t="s">
+        <v>343</v>
+      </c>
+      <c r="D79" t="s">
+        <v>188</v>
+      </c>
+      <c r="E79" t="s">
+        <v>344</v>
+      </c>
+      <c r="F79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G79" t="s">
+        <v>83</v>
+      </c>
+      <c r="H79" t="s">
+        <v>345</v>
+      </c>
+      <c r="J79" t="s">
+        <v>64</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="L79" s="1"/>
+      <c r="M79" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="80" spans="1:24">
       <c r="L80" s="1"/>
@@ -4322,6 +4459,12 @@
     </row>
     <row r="85" spans="12:12">
       <c r="L85" s="1"/>
+    </row>
+    <row r="86" spans="12:12">
+      <c r="L86" s="1"/>
+    </row>
+    <row r="87" spans="12:12">
+      <c r="L87" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>